<commit_message>
Modify UC for active mode, adjust bounds for modal shares
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_ActiveModes.xlsx
+++ b/SuppXLS/Scen_TRA_ActiveModes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB37CFA8-A474-46B3-9252-4FA6BB67C1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7645335-58F1-43C0-A524-C1FF54084D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="142">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -622,17 +622,33 @@
   <si>
     <t xml:space="preserve"> Replacing short car journeys with active modes</t>
   </si>
+  <si>
+    <t>walking</t>
+  </si>
+  <si>
+    <t>cycling</t>
+  </si>
+  <si>
+    <t>TCAR</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +763,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -890,11 +913,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -962,22 +986,28 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1079,13 +1109,13 @@
       <sheetName val="AF"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7">
         <row r="8">
           <cell r="K8" t="str">
@@ -1128,7 +1158,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
+      <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9">
         <row r="4">
           <cell r="C4">
@@ -3396,10 +3426,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5114,8 +5144,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:AQ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5132,99 +5162,86 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="2:43" ht="25.8" customHeight="1">
-      <c r="C3" s="51" t="s">
+    <row r="3" spans="2:43" s="51" customFormat="1" ht="25.8" customHeight="1">
+      <c r="C3" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15"/>
-      <c r="AQ3" s="15"/>
-    </row>
-    <row r="4" spans="2:43" ht="24" customHeight="1">
-      <c r="C4" s="50" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+    </row>
+    <row r="4" spans="2:43" s="51" customFormat="1" ht="24" customHeight="1">
+      <c r="C4" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50" t="s">
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="U4" s="51">
+        <v>2018</v>
+      </c>
+      <c r="V4" s="51">
+        <v>2019</v>
+      </c>
+      <c r="W4" s="51">
+        <v>2020</v>
+      </c>
+      <c r="X4" s="51">
+        <v>2021</v>
+      </c>
+      <c r="Y4" s="51">
+        <v>2022</v>
+      </c>
+      <c r="Z4" s="51">
+        <v>2023</v>
+      </c>
+      <c r="AA4" s="51">
+        <v>2024</v>
+      </c>
+      <c r="AB4" s="51">
+        <v>2025</v>
+      </c>
+      <c r="AC4" s="51">
+        <v>2026</v>
+      </c>
+      <c r="AD4" s="51">
+        <v>2027</v>
+      </c>
+      <c r="AE4" s="51">
+        <v>2028</v>
+      </c>
+      <c r="AF4" s="51">
+        <v>2029</v>
+      </c>
+      <c r="AG4" s="51">
+        <v>2030</v>
+      </c>
     </row>
     <row r="5" spans="2:43">
       <c r="C5" s="15"/>
@@ -5244,20 +5261,61 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
+      <c r="T5" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="U5" s="52">
+        <f>N12</f>
+        <v>0.32377983784854231</v>
+      </c>
+      <c r="V5" s="52">
+        <f>U5+(($AG$5-$U$5)/12)</f>
+        <v>0.34070859991938141</v>
+      </c>
+      <c r="W5" s="52">
+        <f t="shared" ref="W5:AF5" si="0">V5+(($AG$5-$U$5)/12)</f>
+        <v>0.3576373619902205</v>
+      </c>
+      <c r="X5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.3745661240610596</v>
+      </c>
+      <c r="Y5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.3914948861318987</v>
+      </c>
+      <c r="Z5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.4084236482027378</v>
+      </c>
+      <c r="AA5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.4253524102735769</v>
+      </c>
+      <c r="AB5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.442281172344416</v>
+      </c>
+      <c r="AC5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.45920993441525509</v>
+      </c>
+      <c r="AD5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.47613869648609419</v>
+      </c>
+      <c r="AE5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.49306745855693329</v>
+      </c>
+      <c r="AF5" s="52">
+        <f t="shared" si="0"/>
+        <v>0.50999622062777239</v>
+      </c>
+      <c r="AG5" s="52">
+        <f>N13</f>
+        <v>0.52692498269861132</v>
+      </c>
       <c r="AH5" s="15"/>
       <c r="AI5" s="15"/>
       <c r="AJ5" s="15"/>
@@ -5269,7 +5327,63 @@
       <c r="AP5" s="15"/>
       <c r="AQ5" s="15"/>
     </row>
-    <row r="6" spans="2:43" s="15" customFormat="1"/>
+    <row r="6" spans="2:43" s="15" customFormat="1">
+      <c r="T6" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="U6" s="52">
+        <f>N15</f>
+        <v>5.3963306308090382E-2</v>
+      </c>
+      <c r="V6" s="52">
+        <f>U6+(($AG$6-$U$6)/12)</f>
+        <v>5.8460248500431244E-2</v>
+      </c>
+      <c r="W6" s="52">
+        <f t="shared" ref="W6:AF6" si="1">V6+(($AG$6-$U$6)/12)</f>
+        <v>6.2957190692772114E-2</v>
+      </c>
+      <c r="X6" s="52">
+        <f t="shared" si="1"/>
+        <v>6.7454132885112983E-2</v>
+      </c>
+      <c r="Y6" s="52">
+        <f t="shared" si="1"/>
+        <v>7.1951075077453852E-2</v>
+      </c>
+      <c r="Z6" s="52">
+        <f t="shared" si="1"/>
+        <v>7.6448017269794721E-2</v>
+      </c>
+      <c r="AA6" s="52">
+        <f t="shared" si="1"/>
+        <v>8.0944959462135591E-2</v>
+      </c>
+      <c r="AB6" s="52">
+        <f t="shared" si="1"/>
+        <v>8.544190165447646E-2</v>
+      </c>
+      <c r="AC6" s="52">
+        <f t="shared" si="1"/>
+        <v>8.9938843846817329E-2</v>
+      </c>
+      <c r="AD6" s="52">
+        <f t="shared" si="1"/>
+        <v>9.4435786039158198E-2</v>
+      </c>
+      <c r="AE6" s="52">
+        <f t="shared" si="1"/>
+        <v>9.8932728231499067E-2</v>
+      </c>
+      <c r="AF6" s="52">
+        <f t="shared" si="1"/>
+        <v>0.10342967042383994</v>
+      </c>
+      <c r="AG6" s="52">
+        <f>N16</f>
+        <v>0.10792661261618076</v>
+      </c>
+    </row>
     <row r="7" spans="2:43">
       <c r="B7" s="15" t="s">
         <v>25</v>
@@ -5285,26 +5399,67 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
+      <c r="N7" s="50"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="15"/>
+      <c r="T7" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="U7" s="52">
+        <f>N21</f>
+        <v>0.51421690231633799</v>
+      </c>
+      <c r="V7" s="52">
+        <f>U7+(($AG$7-$U$7)/12)</f>
+        <v>0.49279119805315724</v>
+      </c>
+      <c r="W7" s="52">
+        <f t="shared" ref="W7:AF7" si="2">V7+(($AG$7-$U$7)/12)</f>
+        <v>0.4713654937899765</v>
+      </c>
+      <c r="X7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.44993978952679575</v>
+      </c>
+      <c r="Y7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.42851408526361501</v>
+      </c>
+      <c r="Z7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.40708838100043426</v>
+      </c>
+      <c r="AA7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.38566267673725352</v>
+      </c>
+      <c r="AB7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.36423697247407277</v>
+      </c>
+      <c r="AC7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.34281126821089203</v>
+      </c>
+      <c r="AD7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.32138556394771128</v>
+      </c>
+      <c r="AE7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.29995985968453054</v>
+      </c>
+      <c r="AF7" s="52">
+        <f t="shared" si="2"/>
+        <v>0.27853415542134979</v>
+      </c>
+      <c r="AG7" s="52">
+        <f>N22</f>
+        <v>0.25710845115816899</v>
+      </c>
       <c r="AH7" s="15"/>
       <c r="AI7" s="15"/>
       <c r="AJ7" s="15"/>
@@ -5331,7 +5486,7 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
+      <c r="O8" s="50"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
@@ -5768,112 +5923,112 @@
         <v>Walk</v>
       </c>
       <c r="N13" s="29">
-        <f>N12*1.5</f>
-        <v>0.48566975677281343</v>
+        <f>N12*1.627417526057</f>
+        <v>0.52692498269861132</v>
       </c>
       <c r="O13" s="29">
-        <f>O12*1.5</f>
-        <v>0.44309423550077776</v>
+        <f t="shared" ref="O13:AN13" si="3">O12*1.627417526057</f>
+        <v>0.48073288303252903</v>
       </c>
       <c r="P13" s="29">
-        <f>P12*1.5</f>
-        <v>0.52449384659468212</v>
+        <f t="shared" si="3"/>
+        <v>0.56904698550482491</v>
       </c>
       <c r="Q13" s="29">
-        <f>Q12*1.5</f>
-        <v>0.46967039555187051</v>
+        <f t="shared" si="3"/>
+        <v>0.50956655546082519</v>
       </c>
       <c r="R13" s="29">
-        <f>R12*1.5</f>
-        <v>0.45149146286227548</v>
+        <f t="shared" si="3"/>
+        <v>0.48984341301812018</v>
       </c>
       <c r="S13" s="29">
-        <f>S12*1.5</f>
-        <v>0.48878676640595237</v>
+        <f t="shared" si="3"/>
+        <v>0.53030676676918387</v>
       </c>
       <c r="T13" s="29">
-        <f>T12*1.5</f>
-        <v>0.46944134539771509</v>
+        <f t="shared" si="3"/>
+        <v>0.50931804863734609</v>
       </c>
       <c r="U13" s="29">
-        <f>U12*1.5</f>
-        <v>0.5162243990136739</v>
+        <f t="shared" si="3"/>
+        <v>0.56007508955539653</v>
       </c>
       <c r="V13" s="29">
-        <f>V12*1.5</f>
-        <v>0.47460851807783078</v>
+        <f t="shared" si="3"/>
+        <v>0.5149241468905349</v>
       </c>
       <c r="W13" s="29">
-        <f>W12*1.5</f>
-        <v>0.45827846316908699</v>
+        <f t="shared" si="3"/>
+        <v>0.49720693518389303</v>
       </c>
       <c r="X13" s="29">
-        <f>X12*1.5</f>
-        <v>0.46036350190463882</v>
+        <f t="shared" si="3"/>
+        <v>0.49946908757105624</v>
       </c>
       <c r="Y13" s="29">
-        <f>Y12*1.5</f>
-        <v>0.44613036837251807</v>
+        <f t="shared" si="3"/>
+        <v>0.48402692026380101</v>
       </c>
       <c r="Z13" s="29">
-        <f>Z12*1.5</f>
-        <v>0.47977619979092306</v>
+        <f t="shared" si="3"/>
+        <v>0.52053079741651531</v>
       </c>
       <c r="AA13" s="29">
-        <f>AA12*1.5</f>
-        <v>0.45476610507138121</v>
+        <f t="shared" si="3"/>
+        <v>0.49339621976656328</v>
       </c>
       <c r="AB13" s="29">
-        <f>AB12*1.5</f>
-        <v>0.49133729177902113</v>
+        <f t="shared" si="3"/>
+        <v>0.53307394656437401</v>
       </c>
       <c r="AC13" s="29">
-        <f>AC12*1.5</f>
-        <v>0.43663100237891705</v>
+        <f t="shared" si="3"/>
+        <v>0.47372063046085683</v>
       </c>
       <c r="AD13" s="29">
-        <f>AD12*1.5</f>
-        <v>0.48316361222486004</v>
+        <f t="shared" si="3"/>
+        <v>0.52420595365849698</v>
       </c>
       <c r="AE13" s="29">
-        <f>AE12*1.5</f>
-        <v>0.4338622447452814</v>
+        <f t="shared" si="3"/>
+        <v>0.47071668066193501</v>
       </c>
       <c r="AF13" s="29">
-        <f>AF12*1.5</f>
-        <v>0.47574498288192812</v>
+        <f t="shared" si="3"/>
+        <v>0.51615714871715823</v>
       </c>
       <c r="AG13" s="29">
-        <f>AG12*1.5</f>
-        <v>0.47280772521198933</v>
+        <f t="shared" si="3"/>
+        <v>0.51297038564342234</v>
       </c>
       <c r="AH13" s="29">
-        <f>AH12*1.5</f>
-        <v>0.45815741156456141</v>
+        <f t="shared" si="3"/>
+        <v>0.49707560084871821</v>
       </c>
       <c r="AI13" s="29">
-        <f>AI12*1.5</f>
-        <v>0.44648013243648693</v>
+        <f t="shared" si="3"/>
+        <v>0.48440639504225952</v>
       </c>
       <c r="AJ13" s="29">
-        <f>AJ12*1.5</f>
-        <v>0.42211536796751919</v>
+        <f t="shared" si="3"/>
+        <v>0.45797196523222689</v>
       </c>
       <c r="AK13" s="29">
-        <f>AK12*1.5</f>
-        <v>0.48613068014982797</v>
+        <f t="shared" si="3"/>
+        <v>0.52742505921989324</v>
       </c>
       <c r="AL13" s="29">
-        <f>AL12*1.5</f>
-        <v>0.50660267733089259</v>
+        <f t="shared" si="3"/>
+        <v>0.54963605055712927</v>
       </c>
       <c r="AM13" s="29">
-        <f>AM12*1.5</f>
-        <v>0.54576721487657598</v>
+        <f t="shared" si="3"/>
+        <v>0.59212742042497091</v>
       </c>
       <c r="AN13" s="29">
-        <f>AN12*1.5</f>
-        <v>0.43879692647112001</v>
+        <f t="shared" si="3"/>
+        <v>0.47607053901269697</v>
       </c>
       <c r="AO13" s="20">
         <v>0</v>
@@ -6106,103 +6261,103 @@
         <v>9.8465385666839517E-2</v>
       </c>
       <c r="P16" s="29">
-        <f t="shared" ref="P16:AN16" si="0">P15*2</f>
+        <f t="shared" ref="P16:AN16" si="4">P15*2</f>
         <v>0.11655418813215158</v>
       </c>
       <c r="Q16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10437119901152681</v>
       </c>
       <c r="R16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10033143619161676</v>
       </c>
       <c r="S16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10861928142354497</v>
       </c>
       <c r="T16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10432029897727002</v>
       </c>
       <c r="U16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.11471653311414978</v>
       </c>
       <c r="V16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.1054685595728513</v>
       </c>
       <c r="W16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10183965848201933</v>
       </c>
       <c r="X16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10230300042325308</v>
       </c>
       <c r="Y16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.9140081860559601E-2</v>
       </c>
       <c r="Z16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10661693328687179</v>
       </c>
       <c r="AA16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10105913446030694</v>
       </c>
       <c r="AB16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10918606483978248</v>
       </c>
       <c r="AC16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.7029111639759344E-2</v>
       </c>
       <c r="AD16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10736969160552445</v>
       </c>
       <c r="AE16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.6413832165618094E-2</v>
       </c>
       <c r="AF16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10572110730709515</v>
       </c>
       <c r="AG16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10506838338044208</v>
       </c>
       <c r="AH16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10181275812545809</v>
       </c>
       <c r="AI16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.9217807208108202E-2</v>
       </c>
       <c r="AJ16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.3803415103893159E-2</v>
       </c>
       <c r="AK16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.10802904003329514</v>
       </c>
       <c r="AL16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.11257837274019833</v>
       </c>
       <c r="AM16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.12128160330590576</v>
       </c>
       <c r="AN16" s="29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.7510428104693334E-2</v>
       </c>
       <c r="AO16" s="29">
@@ -6279,7 +6434,7 @@
         <v>2018</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L18" s="15">
         <v>-1</v>
@@ -6418,7 +6573,7 @@
         <v>2030</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L19" s="15">
         <v>-1</v>
@@ -6432,111 +6587,111 @@
         <v>1.2024577456126329E-3</v>
       </c>
       <c r="O19" s="29">
-        <f t="shared" ref="O19:AO19" si="1">O18</f>
+        <f t="shared" ref="O19:AO19" si="5">O18</f>
         <v>8.4181954391599476E-4</v>
       </c>
       <c r="P19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4736843073167786E-3</v>
       </c>
       <c r="Q19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.3698908311171865E-3</v>
       </c>
       <c r="R19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.8425388735709995E-4</v>
       </c>
       <c r="S19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.2421004942624992E-4</v>
       </c>
       <c r="T19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2422933671109623E-3</v>
       </c>
       <c r="U19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8.6646068484003841E-4</v>
       </c>
       <c r="V19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.3159890714686659E-3</v>
       </c>
       <c r="W19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2716318220191991E-3</v>
       </c>
       <c r="X19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1218737998245681E-3</v>
       </c>
       <c r="Y19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2891857705150252E-3</v>
       </c>
       <c r="Z19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4574437703184118E-3</v>
       </c>
       <c r="AA19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2419671387040388E-3</v>
       </c>
       <c r="AB19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.4684396048311016E-3</v>
       </c>
       <c r="AC19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.5921086863546602E-4</v>
       </c>
       <c r="AD19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0725657999581929E-3</v>
       </c>
       <c r="AE19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1764845294377178E-3</v>
       </c>
       <c r="AF19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.3287962602263445E-3</v>
       </c>
       <c r="AG19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.9269582890742734E-4</v>
       </c>
       <c r="AH19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AI19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.4007830335184128E-4</v>
       </c>
       <c r="AJ19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.0738302217035411E-4</v>
       </c>
       <c r="AK19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8.0234115950314402E-4</v>
       </c>
       <c r="AL19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.1933080869381386E-4</v>
       </c>
       <c r="AM19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.4164409782466955E-4</v>
       </c>
       <c r="AN19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7.7316749378532367E-4</v>
       </c>
       <c r="AO19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6553,7 +6708,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
@@ -6609,7 +6764,7 @@
         <v>2018</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L21" s="15">
         <v>-1</v>
@@ -6748,7 +6903,7 @@
         <v>2030</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L22" s="15">
         <v>-1</v>
@@ -6762,107 +6917,107 @@
         <v>0.25710845115816899</v>
       </c>
       <c r="O22" s="29">
-        <f t="shared" ref="O22:AN22" si="2">O21*0.5</f>
+        <f t="shared" ref="O22:AN22" si="6">O21*0.5</f>
         <v>0.28848468073825351</v>
       </c>
       <c r="P22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.20759945842607536</v>
       </c>
       <c r="Q22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.2691870581189274</v>
       </c>
       <c r="R22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.26365179492704305</v>
       </c>
       <c r="S22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27214095232329749</v>
       </c>
       <c r="T22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27362209463082626</v>
       </c>
       <c r="U22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.25314740698368299</v>
       </c>
       <c r="V22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27484978119862191</v>
       </c>
       <c r="W22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27143439956463933</v>
       </c>
       <c r="X22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28525400221813491</v>
       </c>
       <c r="Y22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28917008662583377</v>
       </c>
       <c r="Z22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27403883738364437</v>
       </c>
       <c r="AA22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28722775304065862</v>
       </c>
       <c r="AB22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27257079509640914</v>
       </c>
       <c r="AC22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.26471086661485571</v>
       </c>
       <c r="AD22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27445371906158783</v>
       </c>
       <c r="AE22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28827915278858768</v>
       </c>
       <c r="AF22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.2823451425668787</v>
       </c>
       <c r="AG22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.26574494175439495</v>
       </c>
       <c r="AH22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.2855224608280601</v>
       </c>
       <c r="AI22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27231658223640565</v>
       </c>
       <c r="AJ22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.30290341614964916</v>
       </c>
       <c r="AK22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.27287670033140549</v>
       </c>
       <c r="AL22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28565196479848676</v>
       </c>
       <c r="AM22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.28033962298899268</v>
       </c>
       <c r="AN22" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.24642613709310326</v>
       </c>
       <c r="AO22" s="29">
@@ -6882,7 +7037,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
@@ -6938,7 +7093,7 @@
         <v>2018</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L24" s="15">
         <v>-1</v>
@@ -7078,7 +7233,7 @@
         <v>2030</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L25" s="15">
         <v>-1</v>
@@ -7092,107 +7247,107 @@
         <v>1.6399604421517593E-2</v>
       </c>
       <c r="O25" s="29">
-        <f t="shared" ref="O25:AN25" si="3">O24</f>
+        <f t="shared" ref="O25:AN25" si="7">O24</f>
         <v>7.4490307781118984E-3</v>
       </c>
       <c r="P25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.2041705931306341E-2</v>
       </c>
       <c r="Q25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.4142087272297982E-2</v>
       </c>
       <c r="R25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7.8384539751406128E-3</v>
       </c>
       <c r="S25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9.942235039347571E-3</v>
       </c>
       <c r="T25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.7941712391293846E-3</v>
       </c>
       <c r="U25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9167683727598969E-2</v>
       </c>
       <c r="V25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.9563309645198885E-2</v>
       </c>
       <c r="W25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6.7513932047123726E-3</v>
       </c>
       <c r="X25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.1912585101328303E-2</v>
       </c>
       <c r="Y25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6.2742086519266488E-3</v>
       </c>
       <c r="Z25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9.0275647633180547E-3</v>
       </c>
       <c r="AA25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.0257172186811273E-2</v>
       </c>
       <c r="AB25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.2127565539618518E-2</v>
       </c>
       <c r="AC25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.0185353383353699E-2</v>
       </c>
       <c r="AD25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.2812635692286438E-2</v>
       </c>
       <c r="AE25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5.2051948265462115E-3</v>
       </c>
       <c r="AF25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.6226466174633056E-3</v>
       </c>
       <c r="AG25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1.3327262086971724E-2</v>
       </c>
       <c r="AH25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.2106842864435349E-3</v>
       </c>
       <c r="AI25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7.2036254203120672E-3</v>
       </c>
       <c r="AJ25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6.2594387860714779E-3</v>
       </c>
       <c r="AK25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5196368293601697E-3</v>
       </c>
       <c r="AL25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.9112260712667282E-3</v>
       </c>
       <c r="AM25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9.8439085033626087E-3</v>
       </c>
       <c r="AN25" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.1049285439853662E-3</v>
       </c>
       <c r="AO25" s="29">
@@ -7212,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="L26" s="30"/>
       <c r="M26" s="30"/>
@@ -7269,7 +7424,7 @@
         <v>2018</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L27" s="15">
         <v>-1</v>
@@ -7408,7 +7563,7 @@
         <v>2030</v>
       </c>
       <c r="K28" s="32" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L28" s="15">
         <v>-1</v>
@@ -7422,107 +7577,107 @@
         <v>8.2740995898888392E-2</v>
       </c>
       <c r="O28" s="33">
-        <f t="shared" ref="O28:AN28" si="4">O27</f>
+        <f t="shared" ref="O28:AN28" si="8">O27</f>
         <v>7.0110938367526743E-2</v>
       </c>
       <c r="P28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.1139689510378053</v>
       </c>
       <c r="Q28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8.0814709118386313E-2</v>
       </c>
       <c r="R28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.11271367561275741</v>
       </c>
       <c r="S28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.4984165282223824E-2</v>
       </c>
       <c r="T28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.7598299711661989E-2</v>
       </c>
       <c r="U28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.216317572067088E-2</v>
       </c>
       <c r="V28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.0281180381109148E-2</v>
       </c>
       <c r="W28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9.2669371156921962E-2</v>
       </c>
       <c r="X28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.839703518119168E-2</v>
       </c>
       <c r="Y28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.7106145813932178E-2</v>
       </c>
       <c r="Z28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.8278050195023532E-2</v>
       </c>
       <c r="AA28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.0338383982093263E-2</v>
       </c>
       <c r="AB28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.9111177723493433E-2</v>
       </c>
       <c r="AC28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.11983181177914175</v>
       </c>
       <c r="AD28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.1413439765244195E-2</v>
       </c>
       <c r="AE28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.9611602487177441E-2</v>
       </c>
       <c r="AF28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.5334396413720018E-2</v>
       </c>
       <c r="AG28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8.6650816743783748E-2</v>
       </c>
       <c r="AH28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.4399740618333048E-2</v>
       </c>
       <c r="AI28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.10016080657514609</v>
       </c>
       <c r="AJ28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5.8914393028833764E-2</v>
       </c>
       <c r="AK28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.6822981231792783E-2</v>
       </c>
       <c r="AL28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2.5041208932371696E-2</v>
       </c>
       <c r="AM28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.2495898501573662E-3</v>
       </c>
       <c r="AN28" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.16098313140959611</v>
       </c>
       <c r="AO28" s="33">
@@ -7542,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
@@ -7599,7 +7754,7 @@
         <v>2018</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L30" s="15">
         <v>-1</v>
@@ -7739,7 +7894,7 @@
         <v>2030</v>
       </c>
       <c r="K31" s="32" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L31" s="15">
         <v>-1</v>
@@ -7753,107 +7908,107 @@
         <v>7.6968954610109105E-3</v>
       </c>
       <c r="O31" s="33">
-        <f t="shared" ref="O31:AN31" si="5">O30</f>
+        <f t="shared" ref="O31:AN31" si="9">O30</f>
         <v>0</v>
       </c>
       <c r="P31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.9377083408890298E-2</v>
       </c>
       <c r="Q31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AC31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AD31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AG31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AL31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AM31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AN31" s="33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AO31" s="33">
@@ -7873,7 +8028,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
@@ -7921,7 +8076,7 @@
       <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32" t="str">
-        <f t="shared" ref="H33" si="6">H30</f>
+        <f t="shared" ref="H33" si="10">H30</f>
         <v>TRAPS</v>
       </c>
       <c r="I33" s="32"/>
@@ -8082,107 +8237,107 @@
         <v>0</v>
       </c>
       <c r="O34" s="33">
-        <f t="shared" ref="O34:AN34" si="7">O33</f>
+        <f t="shared" ref="O34:AN34" si="11">O33</f>
         <v>0</v>
       </c>
       <c r="P34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Z34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AF34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AH34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AI34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AK34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AL34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AM34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AN34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AO34" s="33">
@@ -9848,7 +10003,7 @@
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32" t="str">
-        <f t="shared" ref="H58" si="8">H56</f>
+        <f t="shared" ref="H58" si="12">H56</f>
         <v>TRAPM</v>
       </c>
       <c r="I58" s="32"/>
@@ -11551,7 +11706,7 @@
       <c r="F83" s="32"/>
       <c r="G83" s="32"/>
       <c r="H83" s="32" t="str">
-        <f t="shared" ref="H83" si="9">H81</f>
+        <f t="shared" ref="H83" si="13">H81</f>
         <v>TRAPL</v>
       </c>
       <c r="I83" s="32"/>

</xml_diff>

<commit_message>
Modify UC for freight transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_ActiveModes.xlsx
+++ b/SuppXLS/Scen_TRA_ActiveModes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\TRA_Update\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B72859-51A2-497B-B131-314AF72C054B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BBD907-F96A-4A86-8320-0D63C29B2911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -976,7 +976,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -984,9 +984,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.000%"/>
     <numFmt numFmtId="173" formatCode="0.00000"/>
   </numFmts>
   <fonts count="28">
@@ -1374,7 +1372,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1477,9 +1475,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1497,18 +1492,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1528,7 +1511,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3288,8 +3283,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:AQ224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N81" sqref="N81"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3307,46 +3302,46 @@
       </c>
     </row>
     <row r="3" spans="2:43" s="35" customFormat="1" ht="25.95" customHeight="1">
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="79" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="83"/>
     </row>
     <row r="4" spans="2:43" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="81" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77" t="s">
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
     </row>
     <row r="5" spans="2:43">
       <c r="C5" s="15"/>
@@ -3551,11 +3546,11 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
@@ -3764,111 +3759,111 @@
         <f>D143</f>
         <v>Walk</v>
       </c>
-      <c r="N12" s="65">
+      <c r="N12" s="62">
         <f>ROUNDUP(C157,3)</f>
         <v>0.32400000000000001</v>
       </c>
-      <c r="O12" s="65">
+      <c r="O12" s="62">
         <f t="shared" ref="O12:AN12" si="0">ROUNDUP(D157,3)</f>
         <v>0.29599999999999999</v>
       </c>
-      <c r="P12" s="65">
+      <c r="P12" s="62">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="Q12" s="65">
+      <c r="Q12" s="62">
         <f t="shared" si="0"/>
         <v>0.314</v>
       </c>
-      <c r="R12" s="65">
+      <c r="R12" s="62">
         <f t="shared" si="0"/>
         <v>0.30099999999999999</v>
       </c>
-      <c r="S12" s="65">
+      <c r="S12" s="62">
         <f t="shared" si="0"/>
         <v>0.32600000000000001</v>
       </c>
-      <c r="T12" s="65">
+      <c r="T12" s="62">
         <f t="shared" si="0"/>
         <v>0.313</v>
       </c>
-      <c r="U12" s="65">
+      <c r="U12" s="62">
         <f t="shared" si="0"/>
         <v>0.34499999999999997</v>
       </c>
-      <c r="V12" s="65">
+      <c r="V12" s="62">
         <f t="shared" si="0"/>
         <v>0.317</v>
       </c>
-      <c r="W12" s="65">
+      <c r="W12" s="62">
         <f t="shared" si="0"/>
         <v>0.30599999999999999</v>
       </c>
-      <c r="X12" s="65">
+      <c r="X12" s="62">
         <f t="shared" si="0"/>
         <v>0.307</v>
       </c>
-      <c r="Y12" s="65">
+      <c r="Y12" s="62">
         <f t="shared" si="0"/>
         <v>0.29799999999999999</v>
       </c>
-      <c r="Z12" s="65">
+      <c r="Z12" s="62">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="AA12" s="65">
+      <c r="AA12" s="62">
         <f t="shared" si="0"/>
         <v>0.30399999999999999</v>
       </c>
-      <c r="AB12" s="65">
+      <c r="AB12" s="62">
         <f t="shared" si="0"/>
         <v>0.32800000000000001</v>
       </c>
-      <c r="AC12" s="65">
+      <c r="AC12" s="62">
         <f t="shared" si="0"/>
         <v>0.29199999999999998</v>
       </c>
-      <c r="AD12" s="65">
+      <c r="AD12" s="62">
         <f t="shared" si="0"/>
         <v>0.32300000000000001</v>
       </c>
-      <c r="AE12" s="65">
+      <c r="AE12" s="62">
         <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="AF12" s="65">
+      <c r="AF12" s="62">
         <f t="shared" si="0"/>
         <v>0.318</v>
       </c>
-      <c r="AG12" s="65">
+      <c r="AG12" s="62">
         <f t="shared" si="0"/>
         <v>0.316</v>
       </c>
-      <c r="AH12" s="65">
+      <c r="AH12" s="62">
         <f t="shared" si="0"/>
         <v>0.30599999999999999</v>
       </c>
-      <c r="AI12" s="65">
+      <c r="AI12" s="62">
         <f t="shared" si="0"/>
         <v>0.29799999999999999</v>
       </c>
-      <c r="AJ12" s="65">
+      <c r="AJ12" s="62">
         <f t="shared" si="0"/>
         <v>0.28200000000000003</v>
       </c>
-      <c r="AK12" s="65">
+      <c r="AK12" s="62">
         <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
-      <c r="AL12" s="65">
+      <c r="AL12" s="62">
         <f t="shared" si="0"/>
         <v>0.33800000000000002</v>
       </c>
-      <c r="AM12" s="65">
+      <c r="AM12" s="62">
         <f t="shared" si="0"/>
         <v>0.36399999999999999</v>
       </c>
-      <c r="AN12" s="65">
+      <c r="AN12" s="62">
         <f t="shared" si="0"/>
         <v>0.29299999999999998</v>
       </c>
@@ -4094,111 +4089,111 @@
         <f>D144</f>
         <v>Bike</v>
       </c>
-      <c r="N15" s="65">
+      <c r="N15" s="62">
         <f>ROUNDUP(C158,3)</f>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="O15" s="65">
+      <c r="O15" s="62">
         <f t="shared" ref="O15:AN15" si="2">ROUNDUP(D158,3)</f>
         <v>0.05</v>
       </c>
-      <c r="P15" s="65">
+      <c r="P15" s="62">
         <f t="shared" si="2"/>
         <v>5.9000000000000004E-2</v>
       </c>
-      <c r="Q15" s="65">
+      <c r="Q15" s="62">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="R15" s="65">
+      <c r="R15" s="62">
         <f t="shared" si="2"/>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="S15" s="65">
+      <c r="S15" s="62">
         <f t="shared" si="2"/>
         <v>5.5E-2</v>
       </c>
-      <c r="T15" s="65">
+      <c r="T15" s="62">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="U15" s="65">
+      <c r="U15" s="62">
         <f t="shared" si="2"/>
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="V15" s="65">
+      <c r="V15" s="62">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="W15" s="65">
+      <c r="W15" s="62">
         <f t="shared" si="2"/>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="X15" s="65">
+      <c r="X15" s="62">
         <f t="shared" si="2"/>
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="Y15" s="65">
+      <c r="Y15" s="62">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="Z15" s="65">
+      <c r="Z15" s="62">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="AA15" s="65">
+      <c r="AA15" s="62">
         <f t="shared" si="2"/>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="AB15" s="65">
+      <c r="AB15" s="62">
         <f t="shared" si="2"/>
         <v>5.5E-2</v>
       </c>
-      <c r="AC15" s="65">
+      <c r="AC15" s="62">
         <f t="shared" si="2"/>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="AD15" s="65">
+      <c r="AD15" s="62">
         <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="AE15" s="65">
+      <c r="AE15" s="62">
         <f t="shared" si="2"/>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="AF15" s="65">
+      <c r="AF15" s="62">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="AG15" s="65">
+      <c r="AG15" s="62">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="AH15" s="65">
+      <c r="AH15" s="62">
         <f t="shared" si="2"/>
         <v>5.1000000000000004E-2</v>
       </c>
-      <c r="AI15" s="65">
+      <c r="AI15" s="62">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="AJ15" s="65">
+      <c r="AJ15" s="62">
         <f t="shared" si="2"/>
         <v>4.7E-2</v>
       </c>
-      <c r="AK15" s="65">
+      <c r="AK15" s="62">
         <f t="shared" si="2"/>
         <v>5.5E-2</v>
       </c>
-      <c r="AL15" s="65">
+      <c r="AL15" s="62">
         <f t="shared" si="2"/>
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="AM15" s="65">
+      <c r="AM15" s="62">
         <f t="shared" si="2"/>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="AN15" s="65">
+      <c r="AN15" s="62">
         <f t="shared" si="2"/>
         <v>4.9000000000000002E-2</v>
       </c>
@@ -4754,111 +4749,111 @@
         <f>D146</f>
         <v>LDV</v>
       </c>
-      <c r="N21" s="65">
+      <c r="N21" s="62">
         <f>ROUNDUP(C160,3)</f>
         <v>0.51500000000000001</v>
       </c>
-      <c r="O21" s="65">
+      <c r="O21" s="62">
         <f t="shared" ref="O21:AN21" si="6">ROUNDUP(D160,3)</f>
         <v>0.57699999999999996</v>
       </c>
-      <c r="P21" s="65">
+      <c r="P21" s="62">
         <f t="shared" si="6"/>
         <v>0.41599999999999998</v>
       </c>
-      <c r="Q21" s="65">
+      <c r="Q21" s="62">
         <f t="shared" si="6"/>
         <v>0.53900000000000003</v>
       </c>
-      <c r="R21" s="65">
+      <c r="R21" s="62">
         <f t="shared" si="6"/>
         <v>0.52800000000000002</v>
       </c>
-      <c r="S21" s="65">
+      <c r="S21" s="62">
         <f t="shared" si="6"/>
         <v>0.54500000000000004</v>
       </c>
-      <c r="T21" s="65">
+      <c r="T21" s="62">
         <f t="shared" si="6"/>
         <v>0.54800000000000004</v>
       </c>
-      <c r="U21" s="65">
+      <c r="U21" s="62">
         <f t="shared" si="6"/>
         <v>0.50700000000000001</v>
       </c>
-      <c r="V21" s="65">
+      <c r="V21" s="62">
         <f t="shared" si="6"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="W21" s="65">
+      <c r="W21" s="62">
         <f t="shared" si="6"/>
         <v>0.54300000000000004</v>
       </c>
-      <c r="X21" s="65">
+      <c r="X21" s="62">
         <f t="shared" si="6"/>
         <v>0.57099999999999995</v>
       </c>
-      <c r="Y21" s="65">
+      <c r="Y21" s="62">
         <f t="shared" si="6"/>
         <v>0.57899999999999996</v>
       </c>
-      <c r="Z21" s="65">
+      <c r="Z21" s="62">
         <f t="shared" si="6"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="AA21" s="65">
+      <c r="AA21" s="62">
         <f t="shared" si="6"/>
         <v>0.57499999999999996</v>
       </c>
-      <c r="AB21" s="65">
+      <c r="AB21" s="62">
         <f t="shared" si="6"/>
         <v>0.54600000000000004</v>
       </c>
-      <c r="AC21" s="65">
+      <c r="AC21" s="62">
         <f t="shared" si="6"/>
         <v>0.53</v>
       </c>
-      <c r="AD21" s="65">
+      <c r="AD21" s="62">
         <f t="shared" si="6"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="AE21" s="65">
+      <c r="AE21" s="62">
         <f t="shared" si="6"/>
         <v>0.57699999999999996</v>
       </c>
-      <c r="AF21" s="65">
+      <c r="AF21" s="62">
         <f t="shared" si="6"/>
         <v>0.56499999999999995</v>
       </c>
-      <c r="AG21" s="65">
+      <c r="AG21" s="62">
         <f t="shared" si="6"/>
         <v>0.53200000000000003</v>
       </c>
-      <c r="AH21" s="65">
+      <c r="AH21" s="62">
         <f t="shared" si="6"/>
         <v>0.57199999999999995</v>
       </c>
-      <c r="AI21" s="65">
+      <c r="AI21" s="62">
         <f t="shared" si="6"/>
         <v>0.54500000000000004</v>
       </c>
-      <c r="AJ21" s="65">
+      <c r="AJ21" s="62">
         <f t="shared" si="6"/>
         <v>0.60599999999999998</v>
       </c>
-      <c r="AK21" s="65">
+      <c r="AK21" s="62">
         <f t="shared" si="6"/>
         <v>0.54600000000000004</v>
       </c>
-      <c r="AL21" s="65">
+      <c r="AL21" s="62">
         <f t="shared" si="6"/>
         <v>0.57199999999999995</v>
       </c>
-      <c r="AM21" s="65">
+      <c r="AM21" s="62">
         <f t="shared" si="6"/>
         <v>0.56100000000000005</v>
       </c>
-      <c r="AN21" s="65">
+      <c r="AN21" s="62">
         <f t="shared" si="6"/>
         <v>0.49299999999999999</v>
       </c>
@@ -5084,111 +5079,111 @@
         <f>D147</f>
         <v>Taxis</v>
       </c>
-      <c r="N24" s="65">
+      <c r="N24" s="62">
         <f>ROUNDUP(C161,3)</f>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="O24" s="65">
+      <c r="O24" s="62">
         <f t="shared" ref="O24:AN24" si="8">ROUNDUP(D161,3)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="P24" s="65">
+      <c r="P24" s="62">
         <f t="shared" si="8"/>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="Q24" s="65">
+      <c r="Q24" s="62">
         <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="R24" s="65">
+      <c r="R24" s="62">
         <f t="shared" si="8"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="S24" s="65">
+      <c r="S24" s="62">
         <f t="shared" si="8"/>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="T24" s="65">
+      <c r="T24" s="62">
         <f t="shared" si="8"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="U24" s="65">
+      <c r="U24" s="62">
         <f t="shared" si="8"/>
         <v>0.02</v>
       </c>
-      <c r="V24" s="65">
+      <c r="V24" s="62">
         <f t="shared" si="8"/>
         <v>0.02</v>
       </c>
-      <c r="W24" s="65">
+      <c r="W24" s="62">
         <f t="shared" si="8"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="X24" s="65">
+      <c r="X24" s="62">
         <f t="shared" si="8"/>
         <v>1.2E-2</v>
       </c>
-      <c r="Y24" s="65">
+      <c r="Y24" s="62">
         <f t="shared" si="8"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Z24" s="65">
+      <c r="Z24" s="62">
         <f t="shared" si="8"/>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="AA24" s="65">
+      <c r="AA24" s="62">
         <f t="shared" si="8"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AB24" s="65">
+      <c r="AB24" s="62">
         <f t="shared" si="8"/>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="AC24" s="65">
+      <c r="AC24" s="62">
         <f t="shared" si="8"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AD24" s="65">
+      <c r="AD24" s="62">
         <f t="shared" si="8"/>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="AE24" s="65">
+      <c r="AE24" s="62">
         <f t="shared" si="8"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AF24" s="65">
+      <c r="AF24" s="62">
         <f t="shared" si="8"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="AG24" s="65">
+      <c r="AG24" s="62">
         <f t="shared" si="8"/>
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="AH24" s="65">
+      <c r="AH24" s="62">
         <f t="shared" si="8"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="AI24" s="65">
+      <c r="AI24" s="62">
         <f t="shared" si="8"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AJ24" s="65">
+      <c r="AJ24" s="62">
         <f t="shared" si="8"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AK24" s="65">
+      <c r="AK24" s="62">
         <f t="shared" si="8"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="AL24" s="65">
+      <c r="AL24" s="62">
         <f t="shared" si="8"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="AM24" s="65">
+      <c r="AM24" s="62">
         <f t="shared" si="8"/>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="AN24" s="65">
+      <c r="AN24" s="62">
         <f t="shared" si="8"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -5414,111 +5409,111 @@
         <f>D148</f>
         <v>BUS</v>
       </c>
-      <c r="N27" s="65">
+      <c r="N27" s="62">
         <f>ROUNDUP(C162,3)</f>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="O27" s="65">
+      <c r="O27" s="62">
         <f t="shared" ref="O27:AN27" si="10">ROUNDUP(D162,3)</f>
         <v>7.1000000000000008E-2</v>
       </c>
-      <c r="P27" s="65">
+      <c r="P27" s="62">
         <f t="shared" si="10"/>
         <v>0.114</v>
       </c>
-      <c r="Q27" s="65">
+      <c r="Q27" s="62">
         <f t="shared" si="10"/>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="R27" s="65">
+      <c r="R27" s="62">
         <f t="shared" si="10"/>
         <v>0.113</v>
       </c>
-      <c r="S27" s="65">
+      <c r="S27" s="62">
         <f t="shared" si="10"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="T27" s="65">
+      <c r="T27" s="62">
         <f t="shared" si="10"/>
         <v>7.8E-2</v>
       </c>
-      <c r="U27" s="65">
+      <c r="U27" s="62">
         <f t="shared" si="10"/>
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="V27" s="65">
+      <c r="V27" s="62">
         <f t="shared" si="10"/>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="W27" s="65">
+      <c r="W27" s="62">
         <f t="shared" si="10"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="X27" s="65">
+      <c r="X27" s="62">
         <f t="shared" si="10"/>
         <v>5.9000000000000004E-2</v>
       </c>
-      <c r="Y27" s="65">
+      <c r="Y27" s="62">
         <f t="shared" si="10"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="Z27" s="65">
+      <c r="Z27" s="62">
         <f t="shared" si="10"/>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="AA27" s="65">
+      <c r="AA27" s="62">
         <f t="shared" si="10"/>
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="AB27" s="65">
+      <c r="AB27" s="62">
         <f t="shared" si="10"/>
         <v>0.06</v>
       </c>
-      <c r="AC27" s="65">
+      <c r="AC27" s="62">
         <f t="shared" si="10"/>
         <v>0.12</v>
       </c>
-      <c r="AD27" s="65">
+      <c r="AD27" s="62">
         <f t="shared" si="10"/>
         <v>6.2E-2</v>
       </c>
-      <c r="AE27" s="65">
+      <c r="AE27" s="62">
         <f t="shared" si="10"/>
         <v>0.08</v>
       </c>
-      <c r="AF27" s="65">
+      <c r="AF27" s="62">
         <f t="shared" si="10"/>
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="AG27" s="65">
+      <c r="AG27" s="62">
         <f t="shared" si="10"/>
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="AH27" s="65">
+      <c r="AH27" s="62">
         <f t="shared" si="10"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="AI27" s="65">
+      <c r="AI27" s="62">
         <f t="shared" si="10"/>
         <v>0.10100000000000001</v>
       </c>
-      <c r="AJ27" s="65">
+      <c r="AJ27" s="62">
         <f t="shared" si="10"/>
         <v>5.9000000000000004E-2</v>
       </c>
-      <c r="AK27" s="65">
+      <c r="AK27" s="62">
         <f t="shared" si="10"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="AL27" s="65">
+      <c r="AL27" s="62">
         <f t="shared" si="10"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AM27" s="65">
+      <c r="AM27" s="62">
         <f t="shared" si="10"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AN27" s="65">
+      <c r="AN27" s="62">
         <f t="shared" si="10"/>
         <v>0.161</v>
       </c>
@@ -5744,111 +5739,111 @@
         <f>D149</f>
         <v>Light rail (LUAS)</v>
       </c>
-      <c r="N30" s="65">
+      <c r="N30" s="62">
         <f>ROUNDUP(C163,3)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="O30" s="65">
+      <c r="O30" s="62">
         <f t="shared" ref="O30:AN30" si="12">ROUNDUP(D163,3)</f>
         <v>0</v>
       </c>
-      <c r="P30" s="65">
+      <c r="P30" s="62">
         <f t="shared" si="12"/>
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="Q30" s="65">
+      <c r="Q30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="R30" s="65">
+      <c r="R30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="S30" s="65">
+      <c r="S30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="T30" s="65">
+      <c r="T30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="U30" s="65">
+      <c r="U30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="V30" s="65">
+      <c r="V30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="W30" s="65">
+      <c r="W30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X30" s="65">
+      <c r="X30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Y30" s="65">
+      <c r="Y30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="65">
+      <c r="Z30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AA30" s="65">
+      <c r="AA30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="65">
+      <c r="AB30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC30" s="65">
+      <c r="AC30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD30" s="65">
+      <c r="AD30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AE30" s="65">
+      <c r="AE30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF30" s="65">
+      <c r="AF30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AG30" s="65">
+      <c r="AG30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AH30" s="65">
+      <c r="AH30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AI30" s="65">
+      <c r="AI30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AJ30" s="65">
+      <c r="AJ30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AK30" s="65">
+      <c r="AK30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AL30" s="65">
+      <c r="AL30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AM30" s="65">
+      <c r="AM30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AN30" s="65">
+      <c r="AN30" s="62">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6102,111 +6097,111 @@
       <c r="M34" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="N34" s="63">
+      <c r="N34" s="60">
         <f>N12+N15+N18+N21+N24+N27+N30</f>
         <v>1.0023</v>
       </c>
-      <c r="O34" s="63">
+      <c r="O34" s="60">
         <f t="shared" ref="O34:AN35" si="14">O12+O15+O18+O21+O24+O27+O30</f>
         <v>1.0028999999999999</v>
       </c>
-      <c r="P34" s="63">
+      <c r="P34" s="60">
         <f t="shared" si="14"/>
         <v>1.0035000000000001</v>
       </c>
-      <c r="Q34" s="63">
+      <c r="Q34" s="60">
         <f t="shared" si="14"/>
         <v>1.0034000000000001</v>
       </c>
-      <c r="R34" s="63">
+      <c r="R34" s="60">
         <f t="shared" si="14"/>
         <v>1.002</v>
       </c>
-      <c r="S34" s="63">
+      <c r="S34" s="60">
         <f t="shared" si="14"/>
         <v>1.0017</v>
       </c>
-      <c r="T34" s="63">
+      <c r="T34" s="60">
         <f t="shared" si="14"/>
         <v>1.0023</v>
       </c>
-      <c r="U34" s="63">
+      <c r="U34" s="60">
         <f t="shared" si="14"/>
         <v>1.0039</v>
       </c>
-      <c r="V34" s="63">
+      <c r="V34" s="60">
         <f t="shared" si="14"/>
         <v>1.0024</v>
       </c>
-      <c r="W34" s="63">
+      <c r="W34" s="60">
         <f t="shared" si="14"/>
         <v>1.0013000000000001</v>
       </c>
-      <c r="X34" s="63">
+      <c r="X34" s="60">
         <f t="shared" si="14"/>
         <v>1.0022</v>
       </c>
-      <c r="Y34" s="63">
+      <c r="Y34" s="60">
         <f t="shared" si="14"/>
         <v>1.0032999999999999</v>
       </c>
-      <c r="Z34" s="63">
+      <c r="Z34" s="60">
         <f t="shared" si="14"/>
         <v>1.0035000000000001</v>
       </c>
-      <c r="AA34" s="63">
+      <c r="AA34" s="60">
         <f t="shared" si="14"/>
         <v>1.0033000000000001</v>
       </c>
-      <c r="AB34" s="63">
+      <c r="AB34" s="60">
         <f t="shared" si="14"/>
         <v>1.0035000000000001</v>
       </c>
-      <c r="AC34" s="63">
+      <c r="AC34" s="60">
         <f t="shared" si="14"/>
         <v>1.0030000000000001</v>
       </c>
-      <c r="AD34" s="63">
+      <c r="AD34" s="60">
         <f t="shared" si="14"/>
         <v>1.0021</v>
       </c>
-      <c r="AE34" s="63">
+      <c r="AE34" s="60">
         <f t="shared" si="14"/>
         <v>1.0031999999999999</v>
       </c>
-      <c r="AF34" s="63">
+      <c r="AF34" s="60">
         <f t="shared" si="14"/>
         <v>1.0024</v>
       </c>
-      <c r="AG34" s="63">
+      <c r="AG34" s="60">
         <f t="shared" si="14"/>
         <v>1.0028000000000001</v>
       </c>
-      <c r="AH34" s="63">
+      <c r="AH34" s="60">
         <f t="shared" si="14"/>
         <v>1.0029999999999999</v>
       </c>
-      <c r="AI34" s="63">
+      <c r="AI34" s="60">
         <f t="shared" si="14"/>
         <v>1.0028000000000001</v>
       </c>
-      <c r="AJ34" s="63">
+      <c r="AJ34" s="60">
         <f t="shared" si="14"/>
         <v>1.0018</v>
       </c>
-      <c r="AK34" s="63">
+      <c r="AK34" s="60">
         <f t="shared" si="14"/>
         <v>1.0029000000000001</v>
       </c>
-      <c r="AL34" s="63">
+      <c r="AL34" s="60">
         <f t="shared" si="14"/>
         <v>1.0027999999999999</v>
       </c>
-      <c r="AM34" s="63">
+      <c r="AM34" s="60">
         <f t="shared" si="14"/>
         <v>1.0018</v>
       </c>
-      <c r="AN34" s="63">
+      <c r="AN34" s="60">
         <f t="shared" si="14"/>
         <v>1.0018</v>
       </c>
@@ -6228,111 +6223,111 @@
       <c r="M35" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="N35" s="63">
+      <c r="N35" s="60">
         <f>N13+N16+N19+N22+N25+N28+N31</f>
         <v>1.0020832784424678</v>
       </c>
-      <c r="O35" s="63">
+      <c r="O35" s="60">
         <f t="shared" ref="O35:U35" si="15">O13+O16+O19+O22+O25+O28+O31</f>
         <v>0.95011558771287197</v>
       </c>
-      <c r="P35" s="63">
+      <c r="P35" s="60">
         <f t="shared" si="15"/>
         <v>1.07409613411995</v>
       </c>
-      <c r="Q35" s="63">
+      <c r="Q35" s="60">
         <f t="shared" si="15"/>
         <v>0.98390910318189795</v>
       </c>
-      <c r="R35" s="63">
+      <c r="R35" s="60">
         <f t="shared" si="15"/>
         <v>0.97785267534315701</v>
       </c>
-      <c r="S35" s="63">
+      <c r="S35" s="60">
         <f t="shared" si="15"/>
         <v>0.98873811349458207</v>
       </c>
-      <c r="T35" s="63">
+      <c r="T35" s="60">
         <f t="shared" si="15"/>
         <v>0.97768168565584102</v>
       </c>
-      <c r="U35" s="63">
+      <c r="U35" s="60">
         <f t="shared" si="15"/>
         <v>1.024859046489665</v>
       </c>
-      <c r="V35" s="63">
+      <c r="V35" s="60">
         <f t="shared" si="14"/>
         <v>0.97929135576006909</v>
       </c>
-      <c r="W35" s="63">
+      <c r="W35" s="60">
         <f t="shared" si="14"/>
         <v>0.972789762973442</v>
       </c>
-      <c r="X35" s="63">
+      <c r="X35" s="60">
         <f t="shared" si="14"/>
         <v>0.96131718049949899</v>
       </c>
-      <c r="Y35" s="63">
+      <c r="Y35" s="60">
         <f t="shared" si="14"/>
         <v>0.95077042276498602</v>
       </c>
-      <c r="Z35" s="63">
+      <c r="Z35" s="60">
         <f t="shared" si="14"/>
         <v>0.98377360833824001</v>
       </c>
-      <c r="AA35" s="63">
+      <c r="AA35" s="60">
         <f t="shared" si="14"/>
         <v>0.95753492792132788</v>
       </c>
-      <c r="AB35" s="63">
+      <c r="AB35" s="60">
         <f t="shared" si="14"/>
         <v>0.99129294854669592</v>
       </c>
-      <c r="AC35" s="63">
+      <c r="AC35" s="60">
         <f t="shared" si="14"/>
         <v>0.97020591760864405</v>
       </c>
-      <c r="AD35" s="63">
+      <c r="AD35" s="60">
         <f t="shared" si="14"/>
         <v>0.98425586091641093</v>
       </c>
-      <c r="AE35" s="63">
+      <c r="AE35" s="60">
         <f t="shared" si="14"/>
         <v>0.94565108255652996</v>
       </c>
-      <c r="AF35" s="63">
+      <c r="AF35" s="60">
         <f t="shared" si="14"/>
         <v>0.97241877328612603</v>
       </c>
-      <c r="AG35" s="63">
+      <c r="AG35" s="60">
         <f t="shared" si="14"/>
         <v>0.98806393823401206</v>
       </c>
-      <c r="AH35" s="63">
+      <c r="AH35" s="60">
         <f t="shared" si="14"/>
         <v>0.95998976297344196</v>
       </c>
-      <c r="AI35" s="63">
+      <c r="AI35" s="60">
         <f t="shared" si="14"/>
         <v>0.96727042276498598</v>
       </c>
-      <c r="AJ35" s="63">
+      <c r="AJ35" s="60">
         <f t="shared" si="14"/>
         <v>0.92273174234807409</v>
       </c>
-      <c r="AK35" s="63">
+      <c r="AK35" s="60">
         <f t="shared" si="14"/>
         <v>0.988810695968525</v>
       </c>
-      <c r="AL35" s="63">
+      <c r="AL35" s="60">
         <f t="shared" si="14"/>
         <v>0.98586712380726615</v>
       </c>
-      <c r="AM35" s="64">
+      <c r="AM35" s="61">
         <f t="shared" si="14"/>
         <v>1.0106799794847479</v>
       </c>
-      <c r="AN35" s="63">
+      <c r="AN35" s="60">
         <f t="shared" si="14"/>
         <v>0.98813333513470114</v>
       </c>
@@ -6604,111 +6599,111 @@
         <f>D145</f>
         <v>2-wheelers</v>
       </c>
-      <c r="N41" s="63">
+      <c r="N41" s="60">
         <f>ROUNDUP(C173,4)</f>
         <v>3.3E-3</v>
       </c>
-      <c r="O41" s="63">
+      <c r="O41" s="60">
         <f t="shared" ref="O41:AN41" si="16">ROUNDUP(D173,4)</f>
         <v>2.1999999999999997E-3</v>
       </c>
-      <c r="P41" s="63">
+      <c r="P41" s="60">
         <f t="shared" si="16"/>
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="Q41" s="63">
+      <c r="Q41" s="60">
         <f t="shared" si="16"/>
         <v>3.6999999999999997E-3</v>
       </c>
-      <c r="R41" s="63">
+      <c r="R41" s="60">
         <f t="shared" si="16"/>
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="S41" s="63">
+      <c r="S41" s="60">
         <f t="shared" si="16"/>
         <v>1.7000000000000001E-3</v>
       </c>
-      <c r="T41" s="63">
+      <c r="T41" s="60">
         <f t="shared" si="16"/>
         <v>3.3E-3</v>
       </c>
-      <c r="U41" s="63">
+      <c r="U41" s="60">
         <f t="shared" si="16"/>
         <v>2.4999999999999996E-3</v>
       </c>
-      <c r="V41" s="63">
+      <c r="V41" s="60">
         <f t="shared" si="16"/>
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="W41" s="63">
+      <c r="W41" s="60">
         <f t="shared" si="16"/>
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="X41" s="63">
+      <c r="X41" s="60">
         <f t="shared" si="16"/>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="Y41" s="63">
+      <c r="Y41" s="60">
         <f t="shared" si="16"/>
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="Z41" s="63">
+      <c r="Z41" s="60">
         <f t="shared" si="16"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AA41" s="63">
+      <c r="AA41" s="60">
         <f t="shared" si="16"/>
         <v>3.3E-3</v>
       </c>
-      <c r="AB41" s="63">
+      <c r="AB41" s="60">
         <f t="shared" si="16"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AC41" s="63">
+      <c r="AC41" s="60">
         <f t="shared" si="16"/>
         <v>2.4999999999999996E-3</v>
       </c>
-      <c r="AD41" s="63">
+      <c r="AD41" s="60">
         <f t="shared" si="16"/>
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="AE41" s="63">
+      <c r="AE41" s="60">
         <f t="shared" si="16"/>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="AF41" s="63">
+      <c r="AF41" s="60">
         <f t="shared" si="16"/>
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="AG41" s="63">
+      <c r="AG41" s="60">
         <f t="shared" si="16"/>
         <v>2.1999999999999997E-3</v>
       </c>
-      <c r="AH41" s="63">
+      <c r="AH41" s="60">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AI41" s="63">
+      <c r="AI41" s="60">
         <f t="shared" si="16"/>
         <v>2E-3</v>
       </c>
-      <c r="AJ41" s="63">
+      <c r="AJ41" s="60">
         <f t="shared" si="16"/>
         <v>1.8E-3</v>
       </c>
-      <c r="AK41" s="63">
+      <c r="AK41" s="60">
         <f t="shared" si="16"/>
         <v>2.1999999999999997E-3</v>
       </c>
-      <c r="AL41" s="63">
+      <c r="AL41" s="60">
         <f t="shared" si="16"/>
         <v>2E-3</v>
       </c>
-      <c r="AM41" s="63">
+      <c r="AM41" s="60">
         <f t="shared" si="16"/>
         <v>2.1999999999999997E-3</v>
       </c>
-      <c r="AN41" s="63">
+      <c r="AN41" s="60">
         <f t="shared" si="16"/>
         <v>2E-3</v>
       </c>
@@ -6779,111 +6774,111 @@
         <f>D146</f>
         <v>LDV</v>
       </c>
-      <c r="N43" s="65">
+      <c r="N43" s="62">
         <f>ROUNDUP(C174,3)</f>
         <v>0.83499999999999996</v>
       </c>
-      <c r="O43" s="65">
+      <c r="O43" s="62">
         <f t="shared" ref="O43:AN43" si="17">ROUNDUP(D174,3)</f>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P43" s="65">
+      <c r="P43" s="62">
         <f t="shared" si="17"/>
         <v>0.72499999999999998</v>
       </c>
-      <c r="Q43" s="65">
+      <c r="Q43" s="62">
         <f t="shared" si="17"/>
         <v>0.85099999999999998</v>
       </c>
-      <c r="R43" s="65">
+      <c r="R43" s="62">
         <f t="shared" si="17"/>
         <v>0.81399999999999995</v>
       </c>
-      <c r="S43" s="65">
+      <c r="S43" s="62">
         <f t="shared" si="17"/>
         <v>0.88100000000000001</v>
       </c>
-      <c r="T43" s="65">
+      <c r="T43" s="62">
         <f t="shared" si="17"/>
         <v>0.86299999999999999</v>
       </c>
-      <c r="U43" s="65">
+      <c r="U43" s="62">
         <f t="shared" si="17"/>
         <v>0.85</v>
       </c>
-      <c r="V43" s="65">
+      <c r="V43" s="62">
         <f t="shared" si="17"/>
         <v>0.875</v>
       </c>
-      <c r="W43" s="65">
+      <c r="W43" s="62">
         <f t="shared" si="17"/>
         <v>0.84399999999999997</v>
       </c>
-      <c r="X43" s="65">
+      <c r="X43" s="62">
         <f t="shared" si="17"/>
         <v>0.89100000000000001</v>
       </c>
-      <c r="Y43" s="65">
+      <c r="Y43" s="62">
         <f t="shared" si="17"/>
         <v>0.88600000000000001</v>
       </c>
-      <c r="Z43" s="65">
+      <c r="Z43" s="62">
         <f t="shared" si="17"/>
         <v>0.876</v>
       </c>
-      <c r="AA43" s="65">
+      <c r="AA43" s="62">
         <f t="shared" si="17"/>
         <v>0.89100000000000001</v>
       </c>
-      <c r="AB43" s="65">
+      <c r="AB43" s="62">
         <f t="shared" si="17"/>
         <v>0.88400000000000001</v>
       </c>
-      <c r="AC43" s="65">
+      <c r="AC43" s="62">
         <f t="shared" si="17"/>
         <v>0.80400000000000005</v>
       </c>
-      <c r="AD43" s="65">
+      <c r="AD43" s="62">
         <f t="shared" si="17"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="AE43" s="65">
+      <c r="AE43" s="62">
         <f t="shared" si="17"/>
         <v>0.871</v>
       </c>
-      <c r="AF43" s="65">
+      <c r="AF43" s="62">
         <f t="shared" si="17"/>
         <v>0.89800000000000002</v>
       </c>
-      <c r="AG43" s="65">
+      <c r="AG43" s="62">
         <f t="shared" si="17"/>
         <v>0.84399999999999997</v>
       </c>
-      <c r="AH43" s="65">
+      <c r="AH43" s="62">
         <f t="shared" si="17"/>
         <v>0.89</v>
       </c>
-      <c r="AI43" s="65">
+      <c r="AI43" s="62">
         <f t="shared" si="17"/>
         <v>0.83599999999999997</v>
       </c>
-      <c r="AJ43" s="65">
+      <c r="AJ43" s="62">
         <f t="shared" si="17"/>
         <v>0.90300000000000002</v>
       </c>
-      <c r="AK43" s="65">
+      <c r="AK43" s="62">
         <f t="shared" si="17"/>
         <v>0.879</v>
       </c>
-      <c r="AL43" s="65">
+      <c r="AL43" s="62">
         <f t="shared" si="17"/>
         <v>0.94499999999999995</v>
       </c>
-      <c r="AM43" s="65">
+      <c r="AM43" s="62">
         <f t="shared" si="17"/>
         <v>0.97699999999999998</v>
       </c>
-      <c r="AN43" s="65">
+      <c r="AN43" s="62">
         <f t="shared" si="17"/>
         <v>0.749</v>
       </c>
@@ -6954,111 +6949,111 @@
         <f>D147</f>
         <v>Taxis</v>
       </c>
-      <c r="N45" s="65">
+      <c r="N45" s="62">
         <f>ROUNDUP(C175,3)</f>
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="O45" s="65">
+      <c r="O45" s="62">
         <f t="shared" ref="O45:AN45" si="18">ROUNDUP(D175,3)</f>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="P45" s="65">
+      <c r="P45" s="62">
         <f t="shared" si="18"/>
         <v>4.7E-2</v>
       </c>
-      <c r="Q45" s="65">
+      <c r="Q45" s="62">
         <f t="shared" si="18"/>
         <v>1.9E-2</v>
       </c>
-      <c r="R45" s="65">
+      <c r="R45" s="62">
         <f t="shared" si="18"/>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="S45" s="65">
+      <c r="S45" s="62">
         <f t="shared" si="18"/>
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="T45" s="65">
+      <c r="T45" s="62">
         <f t="shared" si="18"/>
         <v>1.2E-2</v>
       </c>
-      <c r="U45" s="65">
+      <c r="U45" s="62">
         <f t="shared" si="18"/>
         <v>2.7E-2</v>
       </c>
-      <c r="V45" s="65">
+      <c r="V45" s="62">
         <f t="shared" si="18"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="W45" s="65">
+      <c r="W45" s="62">
         <f t="shared" si="18"/>
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="X45" s="65">
+      <c r="X45" s="62">
         <f t="shared" si="18"/>
         <v>1.6E-2</v>
       </c>
-      <c r="Y45" s="65">
+      <c r="Y45" s="62">
         <f t="shared" si="18"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="Z45" s="65">
+      <c r="Z45" s="62">
         <f t="shared" si="18"/>
         <v>1.2E-2</v>
       </c>
-      <c r="AA45" s="65">
+      <c r="AA45" s="62">
         <f t="shared" si="18"/>
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="AB45" s="65">
+      <c r="AB45" s="62">
         <f t="shared" si="18"/>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AC45" s="65">
+      <c r="AC45" s="62">
         <f t="shared" si="18"/>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="AD45" s="65">
+      <c r="AD45" s="62">
         <f t="shared" si="18"/>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE45" s="65">
+      <c r="AE45" s="62">
         <f t="shared" si="18"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AF45" s="65">
+      <c r="AF45" s="62">
         <f t="shared" si="18"/>
         <v>1.2E-2</v>
       </c>
-      <c r="AG45" s="65">
+      <c r="AG45" s="62">
         <f t="shared" si="18"/>
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="AH45" s="65">
+      <c r="AH45" s="62">
         <f t="shared" si="18"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AI45" s="65">
+      <c r="AI45" s="62">
         <f t="shared" si="18"/>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="AJ45" s="65">
+      <c r="AJ45" s="62">
         <f t="shared" si="18"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AK45" s="65">
+      <c r="AK45" s="62">
         <f t="shared" si="18"/>
         <v>1.2E-2</v>
       </c>
-      <c r="AL45" s="65">
+      <c r="AL45" s="62">
         <f t="shared" si="18"/>
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="AM45" s="65">
+      <c r="AM45" s="62">
         <f t="shared" si="18"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN45" s="65">
+      <c r="AN45" s="62">
         <f t="shared" si="18"/>
         <v>6.0000000000000001E-3</v>
       </c>
@@ -7471,111 +7466,111 @@
       <c r="M52" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="N52" s="63">
+      <c r="N52" s="60">
         <f t="shared" ref="N52:AN52" si="21">SUM(N41:N50)</f>
         <v>1.0103</v>
       </c>
-      <c r="O52" s="63">
+      <c r="O52" s="60">
         <f t="shared" si="21"/>
         <v>1.0042</v>
       </c>
-      <c r="P52" s="63">
+      <c r="P52" s="60">
         <f t="shared" si="21"/>
         <v>1.0064</v>
       </c>
-      <c r="Q52" s="63">
+      <c r="Q52" s="60">
         <f t="shared" si="21"/>
         <v>1.0037</v>
       </c>
-      <c r="R52" s="63">
+      <c r="R52" s="60">
         <f t="shared" si="21"/>
         <v>1.0065999999999999</v>
       </c>
-      <c r="S52" s="63">
+      <c r="S52" s="60">
         <f t="shared" si="21"/>
         <v>1.0067000000000002</v>
       </c>
-      <c r="T52" s="63">
+      <c r="T52" s="60">
         <f t="shared" si="21"/>
         <v>1.0083</v>
       </c>
-      <c r="U52" s="63">
+      <c r="U52" s="60">
         <f t="shared" si="21"/>
         <v>1.0095000000000001</v>
       </c>
-      <c r="V52" s="63">
+      <c r="V52" s="60">
         <f t="shared" si="21"/>
         <v>1.0046000000000002</v>
       </c>
-      <c r="W52" s="63">
+      <c r="W52" s="60">
         <f t="shared" si="21"/>
         <v>1.0064</v>
       </c>
-      <c r="X52" s="63">
+      <c r="X52" s="60">
         <f t="shared" si="21"/>
         <v>1.01</v>
       </c>
-      <c r="Y52" s="63">
+      <c r="Y52" s="60">
         <f t="shared" si="21"/>
         <v>1.0074000000000001</v>
       </c>
-      <c r="Z52" s="63">
+      <c r="Z52" s="60">
         <f t="shared" si="21"/>
         <v>1.002</v>
       </c>
-      <c r="AA52" s="63">
+      <c r="AA52" s="60">
         <f t="shared" si="21"/>
         <v>1.0083</v>
       </c>
-      <c r="AB52" s="63">
+      <c r="AB52" s="60">
         <f t="shared" si="21"/>
         <v>1.0050000000000001</v>
       </c>
-      <c r="AC52" s="63">
+      <c r="AC52" s="60">
         <f t="shared" si="21"/>
         <v>1.0095000000000001</v>
       </c>
-      <c r="AD52" s="63">
+      <c r="AD52" s="60">
         <f t="shared" si="21"/>
         <v>1.0019</v>
       </c>
-      <c r="AE52" s="63">
+      <c r="AE52" s="60">
         <f t="shared" si="21"/>
         <v>1.0110000000000001</v>
       </c>
-      <c r="AF52" s="63">
+      <c r="AF52" s="60">
         <f t="shared" si="21"/>
         <v>1.0036</v>
       </c>
-      <c r="AG52" s="63">
+      <c r="AG52" s="60">
         <f t="shared" si="21"/>
         <v>1.0042</v>
       </c>
-      <c r="AH52" s="63">
+      <c r="AH52" s="60">
         <f t="shared" si="21"/>
         <v>1.0110000000000001</v>
       </c>
-      <c r="AI52" s="63">
+      <c r="AI52" s="60">
         <f t="shared" si="21"/>
         <v>1.008</v>
       </c>
-      <c r="AJ52" s="63">
+      <c r="AJ52" s="60">
         <f t="shared" si="21"/>
         <v>1.0028000000000001</v>
       </c>
-      <c r="AK52" s="63">
+      <c r="AK52" s="60">
         <f t="shared" si="21"/>
         <v>1.0032000000000001</v>
       </c>
-      <c r="AL52" s="63">
+      <c r="AL52" s="60">
         <f t="shared" si="21"/>
         <v>1.01</v>
       </c>
-      <c r="AM52" s="63">
+      <c r="AM52" s="60">
         <f t="shared" si="21"/>
         <v>1.0042</v>
       </c>
-      <c r="AN52" s="63">
+      <c r="AN52" s="60">
         <f t="shared" si="21"/>
         <v>1.0070000000000001</v>
       </c>
@@ -8541,111 +8536,111 @@
       <c r="M69" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="N69" s="63">
+      <c r="N69" s="60">
         <f t="shared" ref="N69:AN69" si="26">SUM(N60:N66)</f>
         <v>1.0150000000000001</v>
       </c>
-      <c r="O69" s="63">
+      <c r="O69" s="60">
         <f t="shared" si="26"/>
         <v>1.0170000000000001</v>
       </c>
-      <c r="P69" s="63">
+      <c r="P69" s="60">
         <f t="shared" si="26"/>
         <v>1.0050000000000001</v>
       </c>
-      <c r="Q69" s="63">
+      <c r="Q69" s="60">
         <f t="shared" si="26"/>
         <v>1.0070000000000001</v>
       </c>
-      <c r="R69" s="63">
+      <c r="R69" s="60">
         <f t="shared" si="26"/>
         <v>1.01</v>
       </c>
-      <c r="S69" s="63">
+      <c r="S69" s="60">
         <f t="shared" si="26"/>
         <v>1.01</v>
       </c>
-      <c r="T69" s="63">
+      <c r="T69" s="60">
         <f t="shared" si="26"/>
         <v>1.004</v>
       </c>
-      <c r="U69" s="63">
+      <c r="U69" s="60">
         <f t="shared" si="26"/>
         <v>1.014</v>
       </c>
-      <c r="V69" s="63">
+      <c r="V69" s="60">
         <f t="shared" si="26"/>
         <v>1.012</v>
       </c>
-      <c r="W69" s="63">
+      <c r="W69" s="60">
         <f t="shared" si="26"/>
         <v>1.0110000000000001</v>
       </c>
-      <c r="X69" s="63">
+      <c r="X69" s="60">
         <f t="shared" si="26"/>
         <v>1.0110000000000001</v>
       </c>
-      <c r="Y69" s="63">
+      <c r="Y69" s="60">
         <f t="shared" si="26"/>
         <v>1.0110000000000001</v>
       </c>
-      <c r="Z69" s="63">
+      <c r="Z69" s="60">
         <f t="shared" si="26"/>
         <v>1.0170000000000001</v>
       </c>
-      <c r="AA69" s="63">
+      <c r="AA69" s="60">
         <f t="shared" si="26"/>
         <v>1.01</v>
       </c>
-      <c r="AB69" s="63">
+      <c r="AB69" s="60">
         <f t="shared" si="26"/>
         <v>1.0090000000000001</v>
       </c>
-      <c r="AC69" s="63">
+      <c r="AC69" s="60">
         <f t="shared" si="26"/>
         <v>1.0029999999999999</v>
       </c>
-      <c r="AD69" s="63">
+      <c r="AD69" s="60">
         <f t="shared" si="26"/>
         <v>1.018</v>
       </c>
-      <c r="AE69" s="63">
+      <c r="AE69" s="60">
         <f t="shared" si="26"/>
         <v>1.014</v>
       </c>
-      <c r="AF69" s="63">
+      <c r="AF69" s="60">
         <f t="shared" si="26"/>
         <v>1.012</v>
       </c>
-      <c r="AG69" s="63">
+      <c r="AG69" s="60">
         <f t="shared" si="26"/>
         <v>1.006</v>
       </c>
-      <c r="AH69" s="63">
+      <c r="AH69" s="60">
         <f t="shared" si="26"/>
         <v>1.012</v>
       </c>
-      <c r="AI69" s="63">
+      <c r="AI69" s="60">
         <f t="shared" si="26"/>
         <v>1.014</v>
       </c>
-      <c r="AJ69" s="63">
+      <c r="AJ69" s="60">
         <f t="shared" si="26"/>
         <v>1.004</v>
       </c>
-      <c r="AK69" s="63">
+      <c r="AK69" s="60">
         <f t="shared" si="26"/>
         <v>1.0170000000000001</v>
       </c>
-      <c r="AL69" s="63">
+      <c r="AL69" s="60">
         <f t="shared" si="26"/>
         <v>1.0190000000000001</v>
       </c>
-      <c r="AM69" s="63">
+      <c r="AM69" s="60">
         <f t="shared" si="26"/>
         <v>1.0090000000000001</v>
       </c>
-      <c r="AN69" s="63">
+      <c r="AN69" s="60">
         <f t="shared" si="26"/>
         <v>1.006</v>
       </c>
@@ -8653,68 +8648,68 @@
       <c r="AP69" s="15"/>
     </row>
     <row r="70" spans="3:42" s="15" customFormat="1">
-      <c r="N70" s="63"/>
-      <c r="O70" s="63"/>
-      <c r="P70" s="63"/>
-      <c r="Q70" s="63"/>
-      <c r="R70" s="63"/>
-      <c r="S70" s="63"/>
-      <c r="T70" s="63"/>
-      <c r="U70" s="63"/>
-      <c r="V70" s="63"/>
-      <c r="W70" s="63"/>
-      <c r="X70" s="63"/>
-      <c r="Y70" s="63"/>
-      <c r="Z70" s="63"/>
-      <c r="AA70" s="63"/>
-      <c r="AB70" s="63"/>
-      <c r="AC70" s="63"/>
-      <c r="AD70" s="63"/>
-      <c r="AE70" s="63"/>
-      <c r="AF70" s="63"/>
-      <c r="AG70" s="63"/>
-      <c r="AH70" s="63"/>
-      <c r="AI70" s="63"/>
-      <c r="AJ70" s="63"/>
-      <c r="AK70" s="63"/>
-      <c r="AL70" s="63"/>
-      <c r="AM70" s="63"/>
-      <c r="AN70" s="63"/>
+      <c r="N70" s="60"/>
+      <c r="O70" s="60"/>
+      <c r="P70" s="60"/>
+      <c r="Q70" s="60"/>
+      <c r="R70" s="60"/>
+      <c r="S70" s="60"/>
+      <c r="T70" s="60"/>
+      <c r="U70" s="60"/>
+      <c r="V70" s="60"/>
+      <c r="W70" s="60"/>
+      <c r="X70" s="60"/>
+      <c r="Y70" s="60"/>
+      <c r="Z70" s="60"/>
+      <c r="AA70" s="60"/>
+      <c r="AB70" s="60"/>
+      <c r="AC70" s="60"/>
+      <c r="AD70" s="60"/>
+      <c r="AE70" s="60"/>
+      <c r="AF70" s="60"/>
+      <c r="AG70" s="60"/>
+      <c r="AH70" s="60"/>
+      <c r="AI70" s="60"/>
+      <c r="AJ70" s="60"/>
+      <c r="AK70" s="60"/>
+      <c r="AL70" s="60"/>
+      <c r="AM70" s="60"/>
+      <c r="AN70" s="60"/>
     </row>
     <row r="71" spans="3:42" s="15" customFormat="1">
-      <c r="N71" s="63"/>
-      <c r="O71" s="63"/>
-      <c r="P71" s="63"/>
-      <c r="Q71" s="63"/>
-      <c r="R71" s="63"/>
-      <c r="S71" s="63"/>
-      <c r="T71" s="63"/>
-      <c r="U71" s="63"/>
-      <c r="V71" s="63"/>
-      <c r="W71" s="63"/>
-      <c r="X71" s="63"/>
-      <c r="Y71" s="63"/>
-      <c r="Z71" s="63"/>
-      <c r="AA71" s="63"/>
-      <c r="AB71" s="63"/>
-      <c r="AC71" s="63"/>
-      <c r="AD71" s="63"/>
-      <c r="AE71" s="63"/>
-      <c r="AF71" s="63"/>
-      <c r="AG71" s="63"/>
-      <c r="AH71" s="63"/>
-      <c r="AI71" s="63"/>
-      <c r="AJ71" s="63"/>
-      <c r="AK71" s="63"/>
-      <c r="AL71" s="63"/>
-      <c r="AM71" s="63"/>
-      <c r="AN71" s="63"/>
+      <c r="N71" s="60"/>
+      <c r="O71" s="60"/>
+      <c r="P71" s="60"/>
+      <c r="Q71" s="60"/>
+      <c r="R71" s="60"/>
+      <c r="S71" s="60"/>
+      <c r="T71" s="60"/>
+      <c r="U71" s="60"/>
+      <c r="V71" s="60"/>
+      <c r="W71" s="60"/>
+      <c r="X71" s="60"/>
+      <c r="Y71" s="60"/>
+      <c r="Z71" s="60"/>
+      <c r="AA71" s="60"/>
+      <c r="AB71" s="60"/>
+      <c r="AC71" s="60"/>
+      <c r="AD71" s="60"/>
+      <c r="AE71" s="60"/>
+      <c r="AF71" s="60"/>
+      <c r="AG71" s="60"/>
+      <c r="AH71" s="60"/>
+      <c r="AI71" s="60"/>
+      <c r="AJ71" s="60"/>
+      <c r="AK71" s="60"/>
+      <c r="AL71" s="60"/>
+      <c r="AM71" s="60"/>
+      <c r="AN71" s="60"/>
     </row>
     <row r="72" spans="3:42" s="15" customFormat="1" ht="18">
-      <c r="C72" s="70" t="s">
+      <c r="C72" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="D72" s="71"/>
+      <c r="D72" s="68"/>
     </row>
     <row r="73" spans="3:42" s="15" customFormat="1"/>
     <row r="74" spans="3:42" s="15" customFormat="1"/>
@@ -8892,115 +8887,115 @@
       <c r="M77" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="N77" s="65">
+      <c r="N77" s="62">
         <f>ROUNDUP(C220,3)</f>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="O77" s="74">
+      <c r="O77" s="71">
         <f t="shared" ref="O77:AN77" si="27">ROUNDUP(D220,3)</f>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="P77" s="74">
+      <c r="P77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="Q77" s="74">
+      <c r="Q77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="R77" s="74">
+      <c r="R77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="S77" s="74">
+      <c r="S77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="T77" s="74">
+      <c r="T77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="U77" s="74">
+      <c r="U77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="V77" s="74">
+      <c r="V77" s="71">
         <f t="shared" si="27"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="W77" s="74">
+      <c r="W77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="X77" s="74">
+      <c r="X77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="Y77" s="74">
+      <c r="Y77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="Z77" s="74">
+      <c r="Z77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AA77" s="74">
+      <c r="AA77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AB77" s="74">
+      <c r="AB77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AC77" s="74">
+      <c r="AC77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AD77" s="74">
+      <c r="AD77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AE77" s="74">
+      <c r="AE77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AF77" s="74">
+      <c r="AF77" s="71">
         <f t="shared" si="27"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AG77" s="74">
+      <c r="AG77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AH77" s="74">
+      <c r="AH77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AI77" s="74">
+      <c r="AI77" s="71">
         <f t="shared" si="27"/>
         <v>2.3E-2</v>
       </c>
-      <c r="AJ77" s="74">
+      <c r="AJ77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AK77" s="74">
+      <c r="AK77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AL77" s="74">
+      <c r="AL77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AM77" s="74">
+      <c r="AM77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AN77" s="74">
+      <c r="AN77" s="71">
         <f t="shared" si="27"/>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="AO77" s="72">
+      <c r="AO77" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9012,32 +9007,32 @@
         <v>66</v>
       </c>
       <c r="N78" s="20"/>
-      <c r="O78" s="73"/>
-      <c r="P78" s="73"/>
-      <c r="Q78" s="73"/>
-      <c r="R78" s="73"/>
-      <c r="S78" s="73"/>
-      <c r="T78" s="73"/>
-      <c r="U78" s="73"/>
-      <c r="V78" s="73"/>
-      <c r="W78" s="73"/>
-      <c r="X78" s="73"/>
-      <c r="Y78" s="73"/>
-      <c r="Z78" s="73"/>
-      <c r="AA78" s="73"/>
-      <c r="AB78" s="73"/>
-      <c r="AC78" s="73"/>
-      <c r="AD78" s="73"/>
-      <c r="AE78" s="73"/>
-      <c r="AF78" s="73"/>
-      <c r="AG78" s="73"/>
-      <c r="AH78" s="73"/>
-      <c r="AI78" s="73"/>
-      <c r="AJ78" s="73"/>
-      <c r="AK78" s="73"/>
-      <c r="AL78" s="73"/>
-      <c r="AM78" s="73"/>
-      <c r="AN78" s="73"/>
+      <c r="O78" s="70"/>
+      <c r="P78" s="70"/>
+      <c r="Q78" s="70"/>
+      <c r="R78" s="70"/>
+      <c r="S78" s="70"/>
+      <c r="T78" s="70"/>
+      <c r="U78" s="70"/>
+      <c r="V78" s="70"/>
+      <c r="W78" s="70"/>
+      <c r="X78" s="70"/>
+      <c r="Y78" s="70"/>
+      <c r="Z78" s="70"/>
+      <c r="AA78" s="70"/>
+      <c r="AB78" s="70"/>
+      <c r="AC78" s="70"/>
+      <c r="AD78" s="70"/>
+      <c r="AE78" s="70"/>
+      <c r="AF78" s="70"/>
+      <c r="AG78" s="70"/>
+      <c r="AH78" s="70"/>
+      <c r="AI78" s="70"/>
+      <c r="AJ78" s="70"/>
+      <c r="AK78" s="70"/>
+      <c r="AL78" s="70"/>
+      <c r="AM78" s="70"/>
+      <c r="AN78" s="70"/>
       <c r="AO78" s="15">
         <v>5</v>
       </c>
@@ -9066,115 +9061,115 @@
       <c r="M79" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="N79" s="65">
+      <c r="N79" s="62">
         <f>ROUNDUP(C221,3)</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="O79" s="74">
+      <c r="O79" s="71">
         <f t="shared" ref="O79:AN79" si="28">ROUNDUP(D221,3)</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="P79" s="74">
+      <c r="P79" s="71">
         <f t="shared" si="28"/>
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="Q79" s="74">
+      <c r="Q79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="R79" s="74">
+      <c r="R79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="S79" s="74">
+      <c r="S79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="T79" s="74">
+      <c r="T79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="U79" s="74">
+      <c r="U79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="V79" s="74">
+      <c r="V79" s="71">
         <f t="shared" si="28"/>
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="W79" s="74">
+      <c r="W79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="X79" s="74">
+      <c r="X79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="Y79" s="74">
+      <c r="Y79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="Z79" s="74">
+      <c r="Z79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AA79" s="74">
+      <c r="AA79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AB79" s="74">
+      <c r="AB79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AC79" s="74">
+      <c r="AC79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AD79" s="74">
+      <c r="AD79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AE79" s="74">
+      <c r="AE79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AF79" s="74">
+      <c r="AF79" s="71">
         <f t="shared" si="28"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AG79" s="74">
+      <c r="AG79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AH79" s="74">
+      <c r="AH79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AI79" s="74">
+      <c r="AI79" s="71">
         <f t="shared" si="28"/>
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="AJ79" s="74">
+      <c r="AJ79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AK79" s="74">
+      <c r="AK79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AL79" s="74">
+      <c r="AL79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AM79" s="74">
+      <c r="AM79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AN79" s="74">
+      <c r="AN79" s="71">
         <f t="shared" si="28"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="AO79" s="72">
+      <c r="AO79" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9186,32 +9181,32 @@
         <v>66</v>
       </c>
       <c r="N80" s="20"/>
-      <c r="O80" s="73"/>
-      <c r="P80" s="73"/>
-      <c r="Q80" s="73"/>
-      <c r="R80" s="73"/>
-      <c r="S80" s="73"/>
-      <c r="T80" s="73"/>
-      <c r="U80" s="73"/>
-      <c r="V80" s="73"/>
-      <c r="W80" s="73"/>
-      <c r="X80" s="73"/>
-      <c r="Y80" s="73"/>
-      <c r="Z80" s="73"/>
-      <c r="AA80" s="73"/>
-      <c r="AB80" s="73"/>
-      <c r="AC80" s="73"/>
-      <c r="AD80" s="73"/>
-      <c r="AE80" s="73"/>
-      <c r="AF80" s="73"/>
-      <c r="AG80" s="73"/>
-      <c r="AH80" s="73"/>
-      <c r="AI80" s="73"/>
-      <c r="AJ80" s="73"/>
-      <c r="AK80" s="73"/>
-      <c r="AL80" s="73"/>
-      <c r="AM80" s="73"/>
-      <c r="AN80" s="73"/>
+      <c r="O80" s="70"/>
+      <c r="P80" s="70"/>
+      <c r="Q80" s="70"/>
+      <c r="R80" s="70"/>
+      <c r="S80" s="70"/>
+      <c r="T80" s="70"/>
+      <c r="U80" s="70"/>
+      <c r="V80" s="70"/>
+      <c r="W80" s="70"/>
+      <c r="X80" s="70"/>
+      <c r="Y80" s="70"/>
+      <c r="Z80" s="70"/>
+      <c r="AA80" s="70"/>
+      <c r="AB80" s="70"/>
+      <c r="AC80" s="70"/>
+      <c r="AD80" s="70"/>
+      <c r="AE80" s="70"/>
+      <c r="AF80" s="70"/>
+      <c r="AG80" s="70"/>
+      <c r="AH80" s="70"/>
+      <c r="AI80" s="70"/>
+      <c r="AJ80" s="70"/>
+      <c r="AK80" s="70"/>
+      <c r="AL80" s="70"/>
+      <c r="AM80" s="70"/>
+      <c r="AN80" s="70"/>
       <c r="AO80" s="15">
         <v>5</v>
       </c>
@@ -9240,115 +9235,115 @@
       <c r="M81" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="N81" s="65">
+      <c r="N81" s="62">
         <f>ROUNDUP(C222,3)</f>
         <v>0.87</v>
       </c>
-      <c r="O81" s="74">
+      <c r="O81" s="71">
         <f t="shared" ref="O81:AN81" si="29">ROUNDUP(D222,3)</f>
         <v>0.876</v>
       </c>
-      <c r="P81" s="74">
+      <c r="P81" s="71">
         <f t="shared" si="29"/>
         <v>0.86699999999999999</v>
       </c>
-      <c r="Q81" s="74">
+      <c r="Q81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="R81" s="74">
+      <c r="R81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="S81" s="74">
+      <c r="S81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="T81" s="74">
+      <c r="T81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="U81" s="74">
+      <c r="U81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="V81" s="74">
+      <c r="V81" s="71">
         <f t="shared" si="29"/>
         <v>0.85699999999999998</v>
       </c>
-      <c r="W81" s="74">
+      <c r="W81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="X81" s="74">
+      <c r="X81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="Y81" s="74">
+      <c r="Y81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="Z81" s="74">
+      <c r="Z81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AA81" s="74">
+      <c r="AA81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AB81" s="74">
+      <c r="AB81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AC81" s="74">
+      <c r="AC81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AD81" s="74">
+      <c r="AD81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AE81" s="74">
+      <c r="AE81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AF81" s="74">
+      <c r="AF81" s="71">
         <f t="shared" si="29"/>
         <v>0.84</v>
       </c>
-      <c r="AG81" s="74">
+      <c r="AG81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AH81" s="74">
+      <c r="AH81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AI81" s="74">
+      <c r="AI81" s="71">
         <f t="shared" si="29"/>
         <v>0.78700000000000003</v>
       </c>
-      <c r="AJ81" s="74">
+      <c r="AJ81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AK81" s="74">
+      <c r="AK81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AL81" s="74">
+      <c r="AL81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AM81" s="74">
+      <c r="AM81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AN81" s="74">
+      <c r="AN81" s="71">
         <f t="shared" si="29"/>
         <v>0.876</v>
       </c>
-      <c r="AO81" s="72">
+      <c r="AO81" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9360,32 +9355,32 @@
         <v>66</v>
       </c>
       <c r="N82" s="20"/>
-      <c r="O82" s="73"/>
-      <c r="P82" s="73"/>
-      <c r="Q82" s="73"/>
-      <c r="R82" s="73"/>
-      <c r="S82" s="73"/>
-      <c r="T82" s="73"/>
-      <c r="U82" s="73"/>
-      <c r="V82" s="73"/>
-      <c r="W82" s="73"/>
-      <c r="X82" s="73"/>
-      <c r="Y82" s="73"/>
-      <c r="Z82" s="73"/>
-      <c r="AA82" s="73"/>
-      <c r="AB82" s="73"/>
-      <c r="AC82" s="73"/>
-      <c r="AD82" s="73"/>
-      <c r="AE82" s="73"/>
-      <c r="AF82" s="73"/>
-      <c r="AG82" s="73"/>
-      <c r="AH82" s="73"/>
-      <c r="AI82" s="73"/>
-      <c r="AJ82" s="73"/>
-      <c r="AK82" s="73"/>
-      <c r="AL82" s="73"/>
-      <c r="AM82" s="73"/>
-      <c r="AN82" s="73"/>
+      <c r="O82" s="70"/>
+      <c r="P82" s="70"/>
+      <c r="Q82" s="70"/>
+      <c r="R82" s="70"/>
+      <c r="S82" s="70"/>
+      <c r="T82" s="70"/>
+      <c r="U82" s="70"/>
+      <c r="V82" s="70"/>
+      <c r="W82" s="70"/>
+      <c r="X82" s="70"/>
+      <c r="Y82" s="70"/>
+      <c r="Z82" s="70"/>
+      <c r="AA82" s="70"/>
+      <c r="AB82" s="70"/>
+      <c r="AC82" s="70"/>
+      <c r="AD82" s="70"/>
+      <c r="AE82" s="70"/>
+      <c r="AF82" s="70"/>
+      <c r="AG82" s="70"/>
+      <c r="AH82" s="70"/>
+      <c r="AI82" s="70"/>
+      <c r="AJ82" s="70"/>
+      <c r="AK82" s="70"/>
+      <c r="AL82" s="70"/>
+      <c r="AM82" s="70"/>
+      <c r="AN82" s="70"/>
       <c r="AO82" s="15">
         <v>5</v>
       </c>
@@ -9414,115 +9409,115 @@
       <c r="M83" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="N83" s="75">
+      <c r="N83" s="72">
         <f>ROUNDUP(C223,3)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="O83" s="75">
+      <c r="O83" s="72">
         <f t="shared" ref="O83:AN83" si="30">ROUNDUP(D223,3)</f>
         <v>0</v>
       </c>
-      <c r="P83" s="75">
+      <c r="P83" s="72">
         <f t="shared" si="30"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="Q83" s="75">
+      <c r="Q83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="R83" s="75">
+      <c r="R83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="S83" s="75">
+      <c r="S83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="T83" s="75">
+      <c r="T83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="U83" s="75">
+      <c r="U83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="V83" s="75">
+      <c r="V83" s="72">
         <f t="shared" si="30"/>
         <v>2.2000000000000002E-2</v>
       </c>
-      <c r="W83" s="75">
+      <c r="W83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="X83" s="75">
+      <c r="X83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="Y83" s="75">
+      <c r="Y83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="Z83" s="75">
+      <c r="Z83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AA83" s="75">
+      <c r="AA83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AB83" s="75">
+      <c r="AB83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AC83" s="75">
+      <c r="AC83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AD83" s="75">
+      <c r="AD83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AE83" s="75">
+      <c r="AE83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AF83" s="75">
+      <c r="AF83" s="72">
         <f t="shared" si="30"/>
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="AG83" s="75">
+      <c r="AG83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AH83" s="75">
+      <c r="AH83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AI83" s="75">
+      <c r="AI83" s="72">
         <f t="shared" si="30"/>
         <v>0.10299999999999999</v>
       </c>
-      <c r="AJ83" s="75">
+      <c r="AJ83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AK83" s="75">
+      <c r="AK83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AL83" s="75">
+      <c r="AL83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AM83" s="75">
+      <c r="AM83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AN83" s="75">
+      <c r="AN83" s="72">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AO83" s="72">
+      <c r="AO83" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9578,143 +9573,143 @@
       <c r="M86" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="N86" s="63">
+      <c r="N86" s="60">
         <f t="shared" ref="N86:AN86" si="31">SUM(N77:N83)</f>
         <v>1.0029999999999999</v>
       </c>
-      <c r="O86" s="63">
+      <c r="O86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="P86" s="63">
+      <c r="P86" s="60">
         <f t="shared" si="31"/>
         <v>1.002</v>
       </c>
-      <c r="Q86" s="63">
+      <c r="Q86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="R86" s="63">
+      <c r="R86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="S86" s="63">
+      <c r="S86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="T86" s="63">
+      <c r="T86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="U86" s="63">
+      <c r="U86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="V86" s="63">
+      <c r="V86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="W86" s="63">
+      <c r="W86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="X86" s="63">
+      <c r="X86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="Y86" s="63">
+      <c r="Y86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="Z86" s="63">
+      <c r="Z86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AA86" s="63">
+      <c r="AA86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AB86" s="63">
+      <c r="AB86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AC86" s="63">
+      <c r="AC86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AD86" s="63">
+      <c r="AD86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AE86" s="63">
+      <c r="AE86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AF86" s="63">
+      <c r="AF86" s="60">
         <f t="shared" si="31"/>
         <v>1.002</v>
       </c>
-      <c r="AG86" s="63">
+      <c r="AG86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AH86" s="63">
+      <c r="AH86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AI86" s="63">
+      <c r="AI86" s="60">
         <f t="shared" si="31"/>
         <v>1.002</v>
       </c>
-      <c r="AJ86" s="63">
+      <c r="AJ86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AK86" s="63">
+      <c r="AK86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AL86" s="63">
+      <c r="AL86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AM86" s="63">
+      <c r="AM86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
-      <c r="AN86" s="63">
+      <c r="AN86" s="60">
         <f t="shared" si="31"/>
         <v>1.0009999999999999</v>
       </c>
     </row>
     <row r="87" spans="3:41" s="15" customFormat="1">
-      <c r="N87" s="63"/>
-      <c r="O87" s="63"/>
-      <c r="P87" s="63"/>
-      <c r="Q87" s="63"/>
-      <c r="R87" s="63"/>
-      <c r="S87" s="63"/>
-      <c r="T87" s="63"/>
-      <c r="U87" s="63"/>
-      <c r="V87" s="63"/>
-      <c r="W87" s="63"/>
-      <c r="X87" s="63"/>
-      <c r="Y87" s="63"/>
-      <c r="Z87" s="63"/>
-      <c r="AA87" s="63"/>
-      <c r="AB87" s="63"/>
-      <c r="AC87" s="63"/>
-      <c r="AD87" s="63"/>
-      <c r="AE87" s="63"/>
-      <c r="AF87" s="63"/>
-      <c r="AG87" s="63"/>
-      <c r="AH87" s="63"/>
-      <c r="AI87" s="63"/>
-      <c r="AJ87" s="63"/>
-      <c r="AK87" s="63"/>
-      <c r="AL87" s="63"/>
-      <c r="AM87" s="63"/>
-      <c r="AN87" s="63"/>
+      <c r="N87" s="60"/>
+      <c r="O87" s="60"/>
+      <c r="P87" s="60"/>
+      <c r="Q87" s="60"/>
+      <c r="R87" s="60"/>
+      <c r="S87" s="60"/>
+      <c r="T87" s="60"/>
+      <c r="U87" s="60"/>
+      <c r="V87" s="60"/>
+      <c r="W87" s="60"/>
+      <c r="X87" s="60"/>
+      <c r="Y87" s="60"/>
+      <c r="Z87" s="60"/>
+      <c r="AA87" s="60"/>
+      <c r="AB87" s="60"/>
+      <c r="AC87" s="60"/>
+      <c r="AD87" s="60"/>
+      <c r="AE87" s="60"/>
+      <c r="AF87" s="60"/>
+      <c r="AG87" s="60"/>
+      <c r="AH87" s="60"/>
+      <c r="AI87" s="60"/>
+      <c r="AJ87" s="60"/>
+      <c r="AK87" s="60"/>
+      <c r="AL87" s="60"/>
+      <c r="AM87" s="60"/>
+      <c r="AN87" s="60"/>
     </row>
     <row r="91" spans="3:41" ht="21">
       <c r="C91" s="45" t="s">
@@ -13307,7 +13302,7 @@
       </c>
     </row>
     <row r="201" spans="1:29">
-      <c r="A201" s="66" t="s">
+      <c r="A201" s="63" t="s">
         <v>231</v>
       </c>
       <c r="B201" s="51" t="s">
@@ -13316,176 +13311,176 @@
       <c r="C201" s="51">
         <v>292</v>
       </c>
-      <c r="D201" s="67">
+      <c r="D201" s="64">
         <v>4.5036639360040285</v>
       </c>
-      <c r="E201" s="67">
+      <c r="E201" s="64">
         <v>66.545424955208503</v>
       </c>
-      <c r="F201" s="67">
+      <c r="F201" s="64">
         <v>12.206547657003652</v>
       </c>
-      <c r="G201" s="67">
+      <c r="G201" s="64">
         <v>7.8498485859894576</v>
       </c>
-      <c r="H201" s="67">
+      <c r="H201" s="64">
         <v>5.5910693087846983</v>
       </c>
-      <c r="I201" s="67">
+      <c r="I201" s="64">
         <v>2.6981330608871263</v>
       </c>
-      <c r="J201" s="67">
+      <c r="J201" s="64">
         <v>7.0705636223405346</v>
       </c>
-      <c r="K201" s="67">
+      <c r="K201" s="64">
         <v>10.700094745319726</v>
       </c>
-      <c r="L201" s="67">
+      <c r="L201" s="64">
         <v>5.146408425117345</v>
       </c>
-      <c r="M201" s="67">
+      <c r="M201" s="64">
         <v>5.8599386346720381</v>
       </c>
-      <c r="N201" s="67">
+      <c r="N201" s="64">
         <v>11.843911540546534</v>
       </c>
-      <c r="O201" s="67">
+      <c r="O201" s="64">
         <v>7.8134215566854737</v>
       </c>
-      <c r="P201" s="67">
+      <c r="P201" s="64">
         <v>7.688817017013525</v>
       </c>
-      <c r="Q201" s="67">
+      <c r="Q201" s="64">
         <v>41.139368114561577</v>
       </c>
-      <c r="R201" s="67">
+      <c r="R201" s="64">
         <v>11.193462584085903</v>
       </c>
-      <c r="S201" s="67">
+      <c r="S201" s="64">
         <v>12.61219141872728</v>
       </c>
-      <c r="T201" s="67">
+      <c r="T201" s="64">
         <v>10.324901499916336</v>
       </c>
-      <c r="U201" s="67">
+      <c r="U201" s="64">
         <v>9.1902209904658907</v>
       </c>
-      <c r="V201" s="67">
+      <c r="V201" s="64">
         <v>15.314016005661671</v>
       </c>
-      <c r="W201" s="67">
+      <c r="W201" s="64">
         <v>2.0423414488510581</v>
       </c>
-      <c r="X201" s="67">
+      <c r="X201" s="64">
         <v>7.7447174156619347</v>
       </c>
-      <c r="Y201" s="67">
+      <c r="Y201" s="64">
         <v>3.830254629073413</v>
       </c>
-      <c r="Z201" s="67">
+      <c r="Z201" s="64">
         <v>4.1769082152806787</v>
       </c>
-      <c r="AA201" s="67">
+      <c r="AA201" s="64">
         <v>4.8551180316963602</v>
       </c>
-      <c r="AB201" s="67">
+      <c r="AB201" s="64">
         <v>10.146187115388139</v>
       </c>
-      <c r="AC201" s="67">
+      <c r="AC201" s="64">
         <v>3.9124694850571404</v>
       </c>
     </row>
     <row r="202" spans="1:29">
-      <c r="A202" s="66" t="s">
+      <c r="A202" s="63" t="s">
         <v>233</v>
       </c>
       <c r="B202" s="51" t="s">
         <v>234</v>
       </c>
-      <c r="C202" s="68">
+      <c r="C202" s="65">
         <v>1140</v>
       </c>
-      <c r="D202" s="67">
+      <c r="D202" s="64">
         <v>17.58279755837189</v>
       </c>
-      <c r="E202" s="67">
+      <c r="E202" s="64">
         <v>259.80063167444416</v>
       </c>
-      <c r="F202" s="67">
+      <c r="F202" s="64">
         <v>47.65569975679508</v>
       </c>
-      <c r="G202" s="67">
+      <c r="G202" s="64">
         <v>30.646669137082128</v>
       </c>
-      <c r="H202" s="67">
+      <c r="H202" s="64">
         <v>21.828147301419712</v>
       </c>
-      <c r="I202" s="67">
+      <c r="I202" s="64">
         <v>10.533807155518234</v>
       </c>
-      <c r="J202" s="67">
+      <c r="J202" s="64">
         <v>27.604255237904827</v>
       </c>
-      <c r="K202" s="67">
+      <c r="K202" s="64">
         <v>41.774342498850984</v>
       </c>
-      <c r="L202" s="67">
+      <c r="L202" s="64">
         <v>20.09214248162251</v>
       </c>
-      <c r="M202" s="67">
+      <c r="M202" s="64">
         <v>22.877842614815492</v>
       </c>
-      <c r="N202" s="67">
+      <c r="N202" s="64">
         <v>46.239928617202224</v>
       </c>
-      <c r="O202" s="67">
+      <c r="O202" s="64">
         <v>30.504454022676164</v>
       </c>
-      <c r="P202" s="67">
+      <c r="P202" s="64">
         <v>30.017984244504856</v>
       </c>
-      <c r="Q202" s="67">
+      <c r="Q202" s="64">
         <v>160.61260154315136</v>
       </c>
-      <c r="R202" s="67">
+      <c r="R202" s="64">
         <v>43.700504609102502</v>
       </c>
-      <c r="S202" s="67">
+      <c r="S202" s="64">
         <v>49.239377456675001</v>
       </c>
-      <c r="T202" s="67">
+      <c r="T202" s="64">
         <v>40.309546951728159</v>
       </c>
-      <c r="U202" s="67">
+      <c r="U202" s="64">
         <v>35.879629894284641</v>
       </c>
-      <c r="V202" s="67">
+      <c r="V202" s="64">
         <v>59.787596734432547</v>
       </c>
-      <c r="W202" s="67">
+      <c r="W202" s="64">
         <v>7.9735248345555005</v>
       </c>
-      <c r="X202" s="67">
+      <c r="X202" s="64">
         <v>30.236225526899336</v>
       </c>
-      <c r="Y202" s="67">
+      <c r="Y202" s="64">
         <v>14.953733825834558</v>
       </c>
-      <c r="Z202" s="67">
+      <c r="Z202" s="64">
         <v>16.307107415821825</v>
       </c>
-      <c r="AA202" s="67">
+      <c r="AA202" s="64">
         <v>18.954912863472092</v>
       </c>
-      <c r="AB202" s="67">
+      <c r="AB202" s="64">
         <v>39.611826409392052</v>
       </c>
-      <c r="AC202" s="67">
+      <c r="AC202" s="64">
         <v>15.27470963344226</v>
       </c>
     </row>
     <row r="203" spans="1:29">
-      <c r="A203" s="66" t="s">
+      <c r="A203" s="63" t="s">
         <v>235</v>
       </c>
       <c r="B203" s="51" t="s">
@@ -13494,169 +13489,169 @@
       <c r="C203" s="51">
         <v>10106</v>
       </c>
-      <c r="D203" s="67">
+      <c r="D203" s="64">
         <v>155.86995800430381</v>
       </c>
-      <c r="E203" s="67">
+      <c r="E203" s="64">
         <v>2303.1098102648534</v>
       </c>
-      <c r="F203" s="67">
+      <c r="F203" s="64">
         <v>422.46359801944828</v>
       </c>
-      <c r="G203" s="67">
+      <c r="G203" s="64">
         <v>271.68003359592279</v>
       </c>
-      <c r="H203" s="67">
+      <c r="H203" s="64">
         <v>193.50461107732247</v>
       </c>
-      <c r="I203" s="67">
+      <c r="I203" s="64">
         <v>93.381276415497609</v>
       </c>
-      <c r="J203" s="67">
+      <c r="J203" s="64">
         <v>244.70930125812822</v>
       </c>
-      <c r="K203" s="67">
+      <c r="K203" s="64">
         <v>370.32588183630531</v>
       </c>
-      <c r="L203" s="67">
+      <c r="L203" s="64">
         <v>178.11508063094482</v>
       </c>
-      <c r="M203" s="67">
+      <c r="M203" s="64">
         <v>202.81006795203979</v>
       </c>
-      <c r="N203" s="67">
+      <c r="N203" s="64">
         <v>409.91291105740851</v>
       </c>
-      <c r="O203" s="67">
+      <c r="O203" s="64">
         <v>270.41930908172395</v>
       </c>
-      <c r="P203" s="67">
+      <c r="P203" s="64">
         <v>266.10679717102289</v>
       </c>
-      <c r="Q203" s="67">
+      <c r="Q203" s="64">
         <v>1423.8166238553399</v>
       </c>
-      <c r="R203" s="67">
+      <c r="R203" s="64">
         <v>387.40113998209637</v>
       </c>
-      <c r="S203" s="67">
+      <c r="S203" s="64">
         <v>436.5027619097873</v>
       </c>
-      <c r="T203" s="67">
+      <c r="T203" s="64">
         <v>357.34059780189892</v>
       </c>
-      <c r="U203" s="67">
+      <c r="U203" s="64">
         <v>318.06977167687774</v>
       </c>
-      <c r="V203" s="67">
+      <c r="V203" s="64">
         <v>530.01180052471523</v>
       </c>
-      <c r="W203" s="67">
+      <c r="W203" s="64">
         <v>70.684598226331474</v>
       </c>
-      <c r="X203" s="67">
+      <c r="X203" s="64">
         <v>268.04148699547778</v>
       </c>
-      <c r="Y203" s="67">
+      <c r="Y203" s="64">
         <v>132.563538634986</v>
       </c>
-      <c r="Z203" s="67">
+      <c r="Z203" s="64">
         <v>144.56107679324157</v>
       </c>
-      <c r="AA203" s="67">
+      <c r="AA203" s="64">
         <v>168.03363982302542</v>
       </c>
-      <c r="AB203" s="67">
+      <c r="AB203" s="64">
         <v>351.15536639764571</v>
       </c>
-      <c r="AC203" s="67">
+      <c r="AC203" s="64">
         <v>135.4089610136557</v>
       </c>
     </row>
     <row r="204" spans="1:29">
-      <c r="A204" s="66" t="s">
+      <c r="A204" s="63" t="s">
         <v>215</v>
       </c>
       <c r="B204" s="51"/>
-      <c r="C204" s="60">
-        <v>8.8551000000000005E-2</v>
-      </c>
-      <c r="D204" s="61">
-        <v>0</v>
-      </c>
-      <c r="E204" s="60">
-        <v>2.8462821428571431E-2</v>
-      </c>
-      <c r="F204" s="62">
-        <v>0</v>
-      </c>
-      <c r="G204" s="62">
-        <v>0</v>
-      </c>
-      <c r="H204" s="62">
-        <v>0</v>
-      </c>
-      <c r="I204" s="62">
-        <v>0</v>
-      </c>
-      <c r="J204" s="62">
-        <v>0</v>
-      </c>
-      <c r="K204" s="60">
-        <v>9.4876071428571431E-3</v>
-      </c>
-      <c r="L204" s="62">
-        <v>0</v>
-      </c>
-      <c r="M204" s="62">
-        <v>0</v>
-      </c>
-      <c r="N204" s="62">
-        <v>0</v>
-      </c>
-      <c r="O204" s="62">
-        <v>0</v>
-      </c>
-      <c r="P204" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q204" s="62">
-        <v>0</v>
-      </c>
-      <c r="R204" s="62">
-        <v>0</v>
-      </c>
-      <c r="S204" s="62">
-        <v>0</v>
-      </c>
-      <c r="T204" s="62">
-        <v>0</v>
-      </c>
-      <c r="U204" s="60">
-        <v>1.5812678571428571E-2</v>
-      </c>
-      <c r="V204" s="62">
-        <v>0</v>
-      </c>
-      <c r="W204" s="62">
-        <v>0</v>
-      </c>
-      <c r="X204" s="60">
-        <v>3.4787892857142858E-2</v>
-      </c>
-      <c r="Y204" s="62">
-        <v>0</v>
-      </c>
-      <c r="Z204" s="62">
-        <v>0</v>
-      </c>
-      <c r="AA204" s="62">
-        <v>0</v>
-      </c>
-      <c r="AB204" s="62">
-        <v>0</v>
-      </c>
-      <c r="AC204" s="62">
+      <c r="C204" s="84">
+        <v>88.551000000000002</v>
+      </c>
+      <c r="D204" s="84">
+        <v>0</v>
+      </c>
+      <c r="E204" s="84">
+        <v>28.462821428571431</v>
+      </c>
+      <c r="F204" s="84">
+        <v>0</v>
+      </c>
+      <c r="G204" s="84">
+        <v>0</v>
+      </c>
+      <c r="H204" s="84">
+        <v>0</v>
+      </c>
+      <c r="I204" s="84">
+        <v>0</v>
+      </c>
+      <c r="J204" s="84">
+        <v>0</v>
+      </c>
+      <c r="K204" s="84">
+        <v>9.4876071428571436</v>
+      </c>
+      <c r="L204" s="84">
+        <v>0</v>
+      </c>
+      <c r="M204" s="84">
+        <v>0</v>
+      </c>
+      <c r="N204" s="84">
+        <v>0</v>
+      </c>
+      <c r="O204" s="84">
+        <v>0</v>
+      </c>
+      <c r="P204" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="84">
+        <v>0</v>
+      </c>
+      <c r="R204" s="84">
+        <v>0</v>
+      </c>
+      <c r="S204" s="84">
+        <v>0</v>
+      </c>
+      <c r="T204" s="84">
+        <v>0</v>
+      </c>
+      <c r="U204" s="84">
+        <v>15.812678571428572</v>
+      </c>
+      <c r="V204" s="84">
+        <v>0</v>
+      </c>
+      <c r="W204" s="84">
+        <v>0</v>
+      </c>
+      <c r="X204" s="84">
+        <v>34.787892857142857</v>
+      </c>
+      <c r="Y204" s="84">
+        <v>0</v>
+      </c>
+      <c r="Z204" s="84">
+        <v>0</v>
+      </c>
+      <c r="AA204" s="84">
+        <v>0</v>
+      </c>
+      <c r="AB204" s="84">
+        <v>0</v>
+      </c>
+      <c r="AC204" s="84">
         <v>0</v>
       </c>
     </row>
@@ -13665,111 +13660,111 @@
       <c r="B205" s="57" t="s">
         <v>216</v>
       </c>
-      <c r="C205" s="69">
+      <c r="C205" s="66">
         <f>SUM(C201:C204)</f>
-        <v>11538.088551000001</v>
-      </c>
-      <c r="D205" s="69">
+        <v>11626.550999999999</v>
+      </c>
+      <c r="D205" s="66">
         <f t="shared" ref="D205:AC205" si="32">SUM(D201:D204)</f>
         <v>177.95641949867974</v>
       </c>
-      <c r="E205" s="69">
+      <c r="E205" s="66">
         <f t="shared" si="32"/>
-        <v>2629.4843297159346</v>
-      </c>
-      <c r="F205" s="69">
+        <v>2657.9186883230773</v>
+      </c>
+      <c r="F205" s="66">
         <f t="shared" si="32"/>
         <v>482.32584543324703</v>
       </c>
-      <c r="G205" s="69">
+      <c r="G205" s="66">
         <f t="shared" si="32"/>
         <v>310.17655131899437</v>
       </c>
-      <c r="H205" s="69">
+      <c r="H205" s="66">
         <f t="shared" si="32"/>
         <v>220.92382768752688</v>
       </c>
-      <c r="I205" s="69">
+      <c r="I205" s="66">
         <f t="shared" si="32"/>
         <v>106.61321663190297</v>
       </c>
-      <c r="J205" s="69">
+      <c r="J205" s="66">
         <f t="shared" si="32"/>
         <v>279.38412011837357</v>
       </c>
-      <c r="K205" s="69">
+      <c r="K205" s="66">
         <f t="shared" si="32"/>
-        <v>422.80980668761885</v>
-      </c>
-      <c r="L205" s="69">
+        <v>432.28792622333316</v>
+      </c>
+      <c r="L205" s="66">
         <f t="shared" si="32"/>
         <v>203.35363153768466</v>
       </c>
-      <c r="M205" s="69">
+      <c r="M205" s="66">
         <f t="shared" si="32"/>
         <v>231.54784920152733</v>
       </c>
-      <c r="N205" s="69">
+      <c r="N205" s="66">
         <f t="shared" si="32"/>
         <v>467.99675121515725</v>
       </c>
-      <c r="O205" s="69">
+      <c r="O205" s="66">
         <f t="shared" si="32"/>
         <v>308.73718466108562</v>
       </c>
-      <c r="P205" s="69">
+      <c r="P205" s="66">
         <f t="shared" si="32"/>
         <v>303.81359843254126</v>
       </c>
-      <c r="Q205" s="69">
+      <c r="Q205" s="66">
         <f t="shared" si="32"/>
         <v>1625.5685935130527</v>
       </c>
-      <c r="R205" s="69">
+      <c r="R205" s="66">
         <f t="shared" si="32"/>
         <v>442.29510717528478</v>
       </c>
-      <c r="S205" s="69">
+      <c r="S205" s="66">
         <f t="shared" si="32"/>
         <v>498.35433078518957</v>
       </c>
-      <c r="T205" s="69">
+      <c r="T205" s="66">
         <f t="shared" si="32"/>
         <v>407.97504625354344</v>
       </c>
-      <c r="U205" s="69">
+      <c r="U205" s="66">
         <f t="shared" si="32"/>
-        <v>363.15543524019967</v>
-      </c>
-      <c r="V205" s="69">
+        <v>378.95230113305684</v>
+      </c>
+      <c r="V205" s="66">
         <f t="shared" si="32"/>
         <v>605.11341326480942</v>
       </c>
-      <c r="W205" s="69">
+      <c r="W205" s="66">
         <f t="shared" si="32"/>
         <v>80.700464509738026</v>
       </c>
-      <c r="X205" s="69">
+      <c r="X205" s="66">
         <f t="shared" si="32"/>
-        <v>306.05721783089621</v>
-      </c>
-      <c r="Y205" s="69">
+        <v>340.81032279518195</v>
+      </c>
+      <c r="Y205" s="66">
         <f t="shared" si="32"/>
         <v>151.34752708989396</v>
       </c>
-      <c r="Z205" s="69">
+      <c r="Z205" s="66">
         <f t="shared" si="32"/>
         <v>165.04509242434406</v>
       </c>
-      <c r="AA205" s="69">
+      <c r="AA205" s="66">
         <f t="shared" si="32"/>
         <v>191.84367071819389</v>
       </c>
-      <c r="AB205" s="69">
+      <c r="AB205" s="66">
         <f t="shared" si="32"/>
         <v>400.91337992242592</v>
       </c>
-      <c r="AC205" s="69">
+      <c r="AC205" s="66">
         <f t="shared" si="32"/>
         <v>154.59614013215509</v>
       </c>
@@ -13808,535 +13803,670 @@
       <c r="AC218" s="15"/>
     </row>
     <row r="219" spans="1:29" ht="17.399999999999999">
-      <c r="A219" s="81" t="s">
+      <c r="A219" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="B219" s="81" t="s">
+      <c r="B219" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="C219" s="82" t="s">
+      <c r="C219" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="D219" s="82" t="s">
+      <c r="D219" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="E219" s="82" t="s">
+      <c r="E219" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F219" s="82" t="s">
+      <c r="F219" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G219" s="82" t="s">
+      <c r="G219" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="H219" s="82" t="s">
+      <c r="H219" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="I219" s="82" t="s">
+      <c r="I219" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="J219" s="82" t="s">
+      <c r="J219" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="K219" s="82" t="s">
+      <c r="K219" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="L219" s="82" t="s">
+      <c r="L219" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="M219" s="82" t="s">
+      <c r="M219" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="N219" s="82" t="s">
+      <c r="N219" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="O219" s="82" t="s">
+      <c r="O219" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="P219" s="82" t="s">
+      <c r="P219" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="Q219" s="82" t="s">
+      <c r="Q219" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="R219" s="82" t="s">
+      <c r="R219" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="S219" s="82" t="s">
+      <c r="S219" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="T219" s="82" t="s">
+      <c r="T219" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="U219" s="82" t="s">
+      <c r="U219" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="V219" s="82" t="s">
+      <c r="V219" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="W219" s="82" t="s">
+      <c r="W219" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="X219" s="82" t="s">
+      <c r="X219" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="Y219" s="82" t="s">
+      <c r="Y219" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="Z219" s="82" t="s">
+      <c r="Z219" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="AA219" s="82" t="s">
+      <c r="AA219" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="AB219" s="82" t="s">
+      <c r="AB219" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="AC219" s="82" t="s">
+      <c r="AC219" s="75" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="220" spans="1:29">
-      <c r="A220" s="86" t="s">
+      <c r="A220" s="79" t="s">
         <v>231</v>
       </c>
-      <c r="B220" s="80" t="s">
+      <c r="B220" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="C220" s="83">
-        <v>2.5114928752301518E-2</v>
-      </c>
-      <c r="D220" s="83">
+      <c r="C220" s="76">
+        <f>C201/C205</f>
+        <v>2.5114928752301521E-2</v>
+      </c>
+      <c r="D220" s="76">
+        <f t="shared" ref="D220:AC220" si="33">D201/D205</f>
         <v>2.5307678973825617E-2</v>
       </c>
-      <c r="E220" s="83">
-        <v>2.5036666940775772E-2</v>
-      </c>
-      <c r="F220" s="83">
+      <c r="E220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5036666940775776E-2</v>
+      </c>
+      <c r="F220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
-      <c r="G220" s="83">
+      <c r="G220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="H220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="I220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825617E-2</v>
+      </c>
+      <c r="J220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="K220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.475224056984587E-2</v>
+      </c>
+      <c r="L220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="M220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825617E-2</v>
+      </c>
+      <c r="N220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825617E-2</v>
+      </c>
+      <c r="O220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825617E-2</v>
+      </c>
+      <c r="P220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="Q220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825624E-2</v>
       </c>
-      <c r="H220" s="83">
+      <c r="R220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
-      <c r="I220" s="83">
+      <c r="S220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825617E-2</v>
+      </c>
+      <c r="T220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="U220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.4251656377299691E-2</v>
+      </c>
+      <c r="V220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="W220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825624E-2</v>
+      </c>
+      <c r="X220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.2724421467469183E-2</v>
+      </c>
+      <c r="Y220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="Z220" s="76">
+        <f t="shared" si="33"/>
+        <v>2.5307678973825621E-2</v>
+      </c>
+      <c r="AA220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825614E-2</v>
       </c>
-      <c r="J220" s="83">
+      <c r="AB220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
-      <c r="K220" s="83">
-        <v>2.475224056984587E-2</v>
-      </c>
-      <c r="L220" s="83">
+      <c r="AC220" s="76">
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
-      <c r="M220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="N220" s="83">
-        <v>2.5307678973825614E-2</v>
-      </c>
-      <c r="O220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="P220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="Q220" s="83">
-        <v>2.5307678973825624E-2</v>
-      </c>
-      <c r="R220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="S220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="T220" s="83">
-        <v>2.5307678973825624E-2</v>
-      </c>
-      <c r="U220" s="83">
-        <v>2.4251656377299691E-2</v>
-      </c>
-      <c r="V220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="W220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="X220" s="83">
-        <v>2.2724421467469186E-2</v>
-      </c>
-      <c r="Y220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="Z220" s="83">
-        <v>2.5307678973825621E-2</v>
-      </c>
-      <c r="AA220" s="83">
-        <v>2.5307678973825614E-2</v>
-      </c>
-      <c r="AB220" s="83">
-        <v>2.5307678973825614E-2</v>
-      </c>
-      <c r="AC220" s="83">
-        <v>2.5307678973825614E-2</v>
-      </c>
     </row>
     <row r="221" spans="1:29">
-      <c r="A221" s="86" t="s">
+      <c r="A221" s="79" t="s">
         <v>233</v>
       </c>
-      <c r="B221" s="80" t="s">
+      <c r="B221" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="C221" s="83">
-        <v>9.8051434169944274E-2</v>
-      </c>
-      <c r="D221" s="83">
+      <c r="C221" s="76">
+        <f>C202/C205</f>
+        <v>9.8051434169944301E-2</v>
+      </c>
+      <c r="D221" s="76">
+        <f t="shared" ref="D221:AC221" si="34">D202/D205</f>
         <v>9.8803952158086308E-2</v>
       </c>
-      <c r="E221" s="83">
-        <v>9.7745891481110903E-2</v>
-      </c>
-      <c r="F221" s="83">
+      <c r="E221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.7745891481110916E-2</v>
+      </c>
+      <c r="F221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="G221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="H221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="I221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="J221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="K221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.663545975898731E-2</v>
+      </c>
+      <c r="L221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="M221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="N221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="O221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="P221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="Q221" s="76">
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
-      <c r="G221" s="83">
+      <c r="R221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="S221" s="76">
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
-      <c r="H221" s="83">
+      <c r="T221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="U221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.4681124212745368E-2</v>
+      </c>
+      <c r="V221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="W221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086336E-2</v>
+      </c>
+      <c r="X221" s="76">
+        <f t="shared" si="34"/>
+        <v>8.8718631756557781E-2</v>
+      </c>
+      <c r="Y221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086336E-2</v>
+      </c>
+      <c r="Z221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086322E-2</v>
+      </c>
+      <c r="AA221" s="76">
+        <f t="shared" si="34"/>
         <v>9.8803952158086308E-2</v>
       </c>
-      <c r="I221" s="83">
+      <c r="AB221" s="76">
+        <f t="shared" si="34"/>
+        <v>9.8803952158086308E-2</v>
+      </c>
+      <c r="AC221" s="76">
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
-      <c r="J221" s="83">
-        <v>9.8803952158086308E-2</v>
-      </c>
-      <c r="K221" s="83">
-        <v>9.663545975898731E-2</v>
-      </c>
-      <c r="L221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="M221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="N221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="O221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="P221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="Q221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="R221" s="83">
-        <v>9.8803952158086336E-2</v>
-      </c>
-      <c r="S221" s="83">
-        <v>9.8803952158086336E-2</v>
-      </c>
-      <c r="T221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="U221" s="83">
-        <v>9.4681124212745368E-2</v>
-      </c>
-      <c r="V221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="W221" s="83">
-        <v>9.8803952158086336E-2</v>
-      </c>
-      <c r="X221" s="83">
-        <v>8.8718631756557781E-2</v>
-      </c>
-      <c r="Y221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="Z221" s="83">
-        <v>9.8803952158086322E-2</v>
-      </c>
-      <c r="AA221" s="83">
-        <v>9.8803952158086308E-2</v>
-      </c>
-      <c r="AB221" s="83">
-        <v>9.8803952158086308E-2</v>
-      </c>
-      <c r="AC221" s="83">
-        <v>9.8803952158086308E-2</v>
-      </c>
     </row>
     <row r="222" spans="1:29">
-      <c r="A222" s="86" t="s">
+      <c r="A222" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="B222" s="80" t="s">
+      <c r="B222" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="C222" s="83">
-        <v>0.86921736291355867</v>
-      </c>
-      <c r="D222" s="83">
+      <c r="C222" s="76">
+        <f>C203/C205</f>
+        <v>0.86921736291355889</v>
+      </c>
+      <c r="D222" s="76">
+        <f t="shared" ref="D222:AC222" si="35">D203/D205</f>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="E222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.86650875377904113</v>
+      </c>
+      <c r="F222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="G222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="H222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="I222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="J222" s="76">
+        <f>J203/J205</f>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="K222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.85666487396870683</v>
+      </c>
+      <c r="L222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="M222" s="76">
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
-      <c r="E222" s="83">
-        <v>0.86650875377904113</v>
-      </c>
-      <c r="F222" s="83">
+      <c r="N222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="O222" s="76">
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
-      <c r="G222" s="83">
+      <c r="P222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="Q222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="R222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="S222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="T222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808796</v>
+      </c>
+      <c r="U222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.83933986078421474</v>
+      </c>
+      <c r="V222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="W222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808807</v>
+      </c>
+      <c r="X222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.78648288818576562</v>
+      </c>
+      <c r="Y222" s="76">
+        <f t="shared" si="35"/>
         <v>0.87588836886808819</v>
       </c>
-      <c r="H222" s="83">
+      <c r="Z222" s="76">
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
-      <c r="I222" s="83">
+      <c r="AA222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808796</v>
+      </c>
+      <c r="AB222" s="76">
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
-      <c r="J222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="K222" s="83">
-        <v>0.85666487396870672</v>
-      </c>
-      <c r="L222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="M222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="N222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="O222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="P222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="Q222" s="83">
-        <v>0.87588836886808796</v>
-      </c>
-      <c r="R222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="S222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="T222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="U222" s="83">
-        <v>0.83933986078421463</v>
-      </c>
-      <c r="V222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="W222" s="83">
-        <v>0.87588836886808796</v>
-      </c>
-      <c r="X222" s="83">
-        <v>0.78648288818576584</v>
-      </c>
-      <c r="Y222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="Z222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="AA222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="AB222" s="83">
-        <v>0.87588836886808807</v>
-      </c>
-      <c r="AC222" s="83">
-        <v>0.87588836886808807</v>
+      <c r="AC222" s="76">
+        <f t="shared" si="35"/>
+        <v>0.87588836886808819</v>
       </c>
     </row>
     <row r="223" spans="1:29">
-      <c r="A223" s="86" t="s">
+      <c r="A223" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="B223" s="80" t="s">
+      <c r="B223" s="73" t="s">
         <v>249</v>
       </c>
-      <c r="C223" s="87">
-        <v>7.6162741641953831E-3</v>
-      </c>
-      <c r="D223" s="87">
-        <v>0</v>
-      </c>
-      <c r="E223" s="87">
-        <v>1.0708687799072239E-2</v>
-      </c>
-      <c r="F223" s="87">
-        <v>0</v>
-      </c>
-      <c r="G223" s="87">
-        <v>0</v>
-      </c>
-      <c r="H223" s="87">
-        <v>0</v>
-      </c>
-      <c r="I223" s="87">
-        <v>0</v>
-      </c>
-      <c r="J223" s="87">
-        <v>0</v>
-      </c>
-      <c r="K223" s="87">
-        <v>2.1947425702460065E-2</v>
-      </c>
-      <c r="L223" s="87">
-        <v>0</v>
-      </c>
-      <c r="M223" s="87">
-        <v>0</v>
-      </c>
-      <c r="N223" s="87">
-        <v>0</v>
-      </c>
-      <c r="O223" s="87">
-        <v>0</v>
-      </c>
-      <c r="P223" s="87">
-        <v>0</v>
-      </c>
-      <c r="Q223" s="87">
-        <v>0</v>
-      </c>
-      <c r="R223" s="87">
-        <v>0</v>
-      </c>
-      <c r="S223" s="87">
-        <v>0</v>
-      </c>
-      <c r="T223" s="87">
-        <v>0</v>
-      </c>
-      <c r="U223" s="87">
+      <c r="C223" s="76">
+        <f>C204/C205</f>
+        <v>7.616274164195384E-3</v>
+      </c>
+      <c r="D223" s="76">
+        <f t="shared" ref="D223:AC223" si="36">D204/D205</f>
+        <v>0</v>
+      </c>
+      <c r="E223" s="76">
+        <f t="shared" si="36"/>
+        <v>1.070868779907224E-2</v>
+      </c>
+      <c r="F223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="H223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="I223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="J223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K223" s="76">
+        <f t="shared" si="36"/>
+        <v>2.1947425702460069E-2</v>
+      </c>
+      <c r="L223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="M223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="N223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="O223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="R223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="S223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="T223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U223" s="76">
+        <f t="shared" si="36"/>
         <v>4.1727358625740237E-2</v>
       </c>
-      <c r="V223" s="87">
-        <v>0</v>
-      </c>
-      <c r="W223" s="87">
-        <v>0</v>
-      </c>
-      <c r="X223" s="87">
+      <c r="V223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="W223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="X223" s="76">
+        <f t="shared" si="36"/>
         <v>0.10207405859020728</v>
       </c>
-      <c r="Y223" s="87">
-        <v>0</v>
-      </c>
-      <c r="Z223" s="87">
-        <v>0</v>
-      </c>
-      <c r="AA223" s="87">
-        <v>0</v>
-      </c>
-      <c r="AB223" s="87">
-        <v>0</v>
-      </c>
-      <c r="AC223" s="87">
+      <c r="Y223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Z223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AA223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AB223" s="76">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AC223" s="76">
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:29">
-      <c r="A224" s="84"/>
-      <c r="B224" s="84" t="s">
+      <c r="A224" s="77"/>
+      <c r="B224" s="77" t="s">
         <v>216</v>
       </c>
-      <c r="C224" s="85">
+      <c r="C224" s="78">
+        <f>SUM(C220:C223)</f>
+        <v>1</v>
+      </c>
+      <c r="D224" s="78">
+        <f t="shared" ref="D224:AC224" si="37">SUM(D220:D223)</f>
+        <v>1</v>
+      </c>
+      <c r="E224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="F224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="G224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="H224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="I224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="J224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="K224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="L224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="M224" s="78">
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="D224" s="85">
+      <c r="N224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="O224" s="78">
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="E224" s="85">
+      <c r="P224" s="78">
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="F224" s="85">
+      <c r="Q224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="R224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="S224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="T224" s="78">
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="G224" s="85">
+      <c r="U224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="V224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="W224" s="78">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="X224" s="78">
+        <f t="shared" si="37"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="Y224" s="78">
+        <f t="shared" si="37"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="H224" s="85">
+      <c r="Z224" s="78">
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="I224" s="85">
+      <c r="AA224" s="78">
+        <f t="shared" si="37"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="AB224" s="78">
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="J224" s="85">
-        <v>1</v>
-      </c>
-      <c r="K224" s="85">
-        <v>1</v>
-      </c>
-      <c r="L224" s="85">
-        <v>1</v>
-      </c>
-      <c r="M224" s="85">
-        <v>1</v>
-      </c>
-      <c r="N224" s="85">
-        <v>1</v>
-      </c>
-      <c r="O224" s="85">
-        <v>1</v>
-      </c>
-      <c r="P224" s="85">
-        <v>1</v>
-      </c>
-      <c r="Q224" s="85">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="R224" s="85">
-        <v>1</v>
-      </c>
-      <c r="S224" s="85">
-        <v>1</v>
-      </c>
-      <c r="T224" s="85">
-        <v>1</v>
-      </c>
-      <c r="U224" s="85">
-        <v>1</v>
-      </c>
-      <c r="V224" s="85">
-        <v>1</v>
-      </c>
-      <c r="W224" s="85">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="X224" s="85">
-        <v>1</v>
-      </c>
-      <c r="Y224" s="85">
-        <v>1</v>
-      </c>
-      <c r="Z224" s="85">
-        <v>1</v>
-      </c>
-      <c r="AA224" s="85">
-        <v>1</v>
-      </c>
-      <c r="AB224" s="85">
-        <v>1</v>
-      </c>
-      <c r="AC224" s="85">
-        <v>1</v>
+      <c r="AC224" s="78">
+        <f t="shared" si="37"/>
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify UC and Load factor for goods vehicle
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_ActiveModes.xlsx
+++ b/SuppXLS/Scen_TRA_ActiveModes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39916E61-861A-40F1-BC30-1101F1E79DBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D166B2F-79B6-42D4-95D3-BE7ABAD557BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="251">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -969,18 +969,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>FX</t>
-  </si>
-  <si>
-    <t>T-LGT*</t>
-  </si>
-  <si>
-    <t>T-MGT*</t>
-  </si>
-  <si>
-    <t>T-HGT*</t>
   </si>
   <si>
     <t>T-GTR*</t>
@@ -1408,7 +1396,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1546,20 +1534,10 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1573,6 +1551,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -3235,8 +3216,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:AQ224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N81" sqref="N81"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3254,46 +3235,46 @@
       </c>
     </row>
     <row r="3" spans="2:43" s="35" customFormat="1" ht="25.95" customHeight="1">
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="96" t="s">
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="96"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="2:43" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94" t="s">
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
     </row>
     <row r="5" spans="2:43">
       <c r="C5" s="15"/>
@@ -3498,11 +3479,11 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="93" t="s">
+      <c r="K10" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="93"/>
-      <c r="M10" s="93"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
@@ -8667,1044 +8648,1103 @@
     <row r="73" spans="3:42" s="15" customFormat="1"/>
     <row r="74" spans="3:42" s="15" customFormat="1"/>
     <row r="75" spans="3:42" s="15" customFormat="1">
-      <c r="C75" s="84"/>
-      <c r="D75" s="84"/>
-      <c r="E75" s="84"/>
-      <c r="F75" s="84"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="84"/>
-      <c r="I75" s="84"/>
-      <c r="J75" s="84"/>
-      <c r="K75" s="84" t="s">
+      <c r="C75" s="81"/>
+      <c r="D75" s="81"/>
+      <c r="E75" s="81"/>
+      <c r="F75" s="81"/>
+      <c r="G75" s="81"/>
+      <c r="H75" s="81"/>
+      <c r="I75" s="81"/>
+      <c r="J75" s="81"/>
+      <c r="K75" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="L75" s="84"/>
-      <c r="M75" s="84"/>
-      <c r="N75" s="84"/>
-      <c r="O75" s="84"/>
-      <c r="P75" s="84"/>
-      <c r="Q75" s="84"/>
-      <c r="R75" s="84"/>
-      <c r="S75" s="84"/>
-      <c r="T75" s="84"/>
-      <c r="U75" s="84"/>
-      <c r="V75" s="84"/>
-      <c r="W75" s="84"/>
-      <c r="X75" s="84"/>
-      <c r="Y75" s="84"/>
-      <c r="Z75" s="84"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="84"/>
-      <c r="AC75" s="84"/>
-      <c r="AD75" s="84"/>
-      <c r="AE75" s="84"/>
-      <c r="AF75" s="84"/>
-      <c r="AG75" s="84"/>
-      <c r="AH75" s="84"/>
-      <c r="AI75" s="84"/>
-      <c r="AJ75" s="84"/>
-      <c r="AK75" s="84"/>
-      <c r="AL75" s="84"/>
-      <c r="AM75" s="84"/>
-      <c r="AN75" s="84"/>
-      <c r="AO75" s="84"/>
+      <c r="L75" s="81"/>
+      <c r="M75" s="81"/>
+      <c r="N75" s="81"/>
+      <c r="O75" s="81"/>
+      <c r="P75" s="81"/>
+      <c r="Q75" s="81"/>
+      <c r="R75" s="81"/>
+      <c r="S75" s="81"/>
+      <c r="T75" s="81"/>
+      <c r="U75" s="81"/>
+      <c r="V75" s="81"/>
+      <c r="W75" s="81"/>
+      <c r="X75" s="81"/>
+      <c r="Y75" s="81"/>
+      <c r="Z75" s="81"/>
+      <c r="AA75" s="81"/>
+      <c r="AB75" s="81"/>
+      <c r="AC75" s="81"/>
+      <c r="AD75" s="81"/>
+      <c r="AE75" s="81"/>
+      <c r="AF75" s="81"/>
+      <c r="AG75" s="81"/>
+      <c r="AH75" s="81"/>
+      <c r="AI75" s="81"/>
+      <c r="AJ75" s="81"/>
+      <c r="AK75" s="81"/>
+      <c r="AL75" s="81"/>
+      <c r="AM75" s="81"/>
+      <c r="AN75" s="81"/>
+      <c r="AO75" s="81"/>
     </row>
     <row r="76" spans="3:42" s="15" customFormat="1">
-      <c r="C76" s="81" t="s">
+      <c r="C76" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D76" s="79" t="s">
+      <c r="D76" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="79" t="s">
+      <c r="E76" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="79" t="s">
+      <c r="F76" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G76" s="79" t="s">
+      <c r="G76" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H76" s="80" t="s">
+      <c r="H76" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I76" s="80" t="s">
+      <c r="I76" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J76" s="80" t="s">
+      <c r="J76" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K76" s="80" t="s">
+      <c r="K76" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L76" s="80" t="s">
+      <c r="L76" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M76" s="81" t="s">
+      <c r="M76" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="N76" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="O76" s="82" t="s">
-        <v>90</v>
-      </c>
-      <c r="P76" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q76" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="R76" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="S76" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="T76" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="U76" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="V76" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="W76" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="X76" s="82" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y76" s="82" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z76" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA76" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB76" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC76" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD76" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE76" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF76" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG76" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH76" s="82" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI76" s="82" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ76" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK76" s="82" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL76" s="82" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM76" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN76" s="82" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO76" s="81" t="s">
+      <c r="N76" s="79" t="str">
+        <f>Regions!C$3</f>
+        <v>IE</v>
+      </c>
+      <c r="O76" s="79" t="str">
+        <f>Regions!D$3</f>
+        <v>National</v>
+      </c>
+      <c r="P76" s="79" t="str">
+        <f>Regions!E$3</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="Q76" s="79" t="str">
+        <f>Regions!F$3</f>
+        <v>IE-D</v>
+      </c>
+      <c r="R76" s="79" t="str">
+        <f>Regions!G$3</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="S76" s="79" t="str">
+        <f>Regions!H$3</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="T76" s="79" t="str">
+        <f>Regions!I$3</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="U76" s="79" t="str">
+        <f>Regions!J$3</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="V76" s="79" t="str">
+        <f>Regions!K$3</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="W76" s="79" t="str">
+        <f>Regions!L$3</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="X76" s="79" t="str">
+        <f>Regions!M$3</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="Y76" s="79" t="str">
+        <f>Regions!N$3</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="Z76" s="79" t="str">
+        <f>Regions!O$3</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="AA76" s="79" t="str">
+        <f>Regions!P$3</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="AB76" s="79" t="str">
+        <f>Regions!Q$3</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="AC76" s="79" t="str">
+        <f>Regions!R$3</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="AD76" s="79" t="str">
+        <f>Regions!S$3</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="AE76" s="79" t="str">
+        <f>Regions!T$3</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="AF76" s="79" t="str">
+        <f>Regions!U$3</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="AG76" s="79" t="str">
+        <f>Regions!V$3</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="AH76" s="79" t="str">
+        <f>Regions!W$3</f>
+        <v>IE-G</v>
+      </c>
+      <c r="AI76" s="79" t="str">
+        <f>Regions!X$3</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="AJ76" s="79" t="str">
+        <f>Regions!Y$3</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="AK76" s="79" t="str">
+        <f>Regions!Z$3</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AL76" s="79" t="str">
+        <f>Regions!AA$3</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AM76" s="79" t="str">
+        <f>Regions!AB$3</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AN76" s="79" t="str">
+        <f>Regions!AC$3</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AO76" s="79" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="77" spans="3:42" s="15" customFormat="1">
-      <c r="C77" s="84" t="s">
+      <c r="C77" s="78" t="s">
         <v>238</v>
       </c>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84" t="s">
-        <v>251</v>
-      </c>
-      <c r="F77" s="84"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="84" t="s">
+      <c r="D77" s="78"/>
+      <c r="E77" s="78" t="str">
+        <f>LEFT(C121,5)&amp;"*"</f>
+        <v>T-LGT*</v>
+      </c>
+      <c r="F77" s="78"/>
+      <c r="G77" s="78"/>
+      <c r="H77" s="78" t="s">
         <v>246</v>
       </c>
-      <c r="I77" s="84"/>
+      <c r="I77" s="78"/>
       <c r="J77" s="78">
         <v>2018</v>
       </c>
       <c r="K77" s="78" t="s">
-        <v>250</v>
-      </c>
-      <c r="L77" s="84">
+        <v>122</v>
+      </c>
+      <c r="L77" s="78">
         <v>-1</v>
       </c>
-      <c r="M77" s="84" t="s">
+      <c r="M77" s="78" t="s">
         <v>239</v>
       </c>
-      <c r="N77" s="88">
-        <f>ROUNDUP(C220,5)</f>
-        <v>2.512E-2</v>
-      </c>
-      <c r="O77" s="88">
-        <f t="shared" ref="O77:AN77" si="27">ROUNDUP(D220,5)</f>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="P77" s="88">
+      <c r="N77" s="89">
+        <f>ROUNDDOWN(C220,5)</f>
+        <v>2.511E-2</v>
+      </c>
+      <c r="O77" s="89">
+        <f t="shared" ref="O77:AN77" si="27">ROUNDDOWN(D220,5)</f>
+        <v>2.53E-2</v>
+      </c>
+      <c r="P77" s="89">
         <f t="shared" si="27"/>
-        <v>2.504E-2</v>
-      </c>
-      <c r="Q77" s="88">
+        <v>2.503E-2</v>
+      </c>
+      <c r="Q77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="R77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="R77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="S77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="S77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="T77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="T77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="U77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="U77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="V77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="V77" s="89">
         <f t="shared" si="27"/>
-        <v>2.4760000000000001E-2</v>
-      </c>
-      <c r="W77" s="88">
+        <v>2.4750000000000001E-2</v>
+      </c>
+      <c r="W77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="X77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="X77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="Y77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="Y77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="Z77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="Z77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AA77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AA77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AB77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AB77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AC77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AC77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AD77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AD77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AE77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AE77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AF77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AF77" s="89">
         <f t="shared" si="27"/>
-        <v>2.426E-2</v>
-      </c>
-      <c r="AG77" s="88">
+        <v>2.4250000000000001E-2</v>
+      </c>
+      <c r="AG77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AH77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AH77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AI77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AI77" s="89">
         <f t="shared" si="27"/>
-        <v>2.273E-2</v>
-      </c>
-      <c r="AJ77" s="88">
+        <v>2.2720000000000001E-2</v>
+      </c>
+      <c r="AJ77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AK77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AK77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AL77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AL77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AM77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AM77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AN77" s="88">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AN77" s="89">
         <f t="shared" si="27"/>
-        <v>2.5309999999999999E-2</v>
-      </c>
-      <c r="AO77" s="90">
+        <v>2.53E-2</v>
+      </c>
+      <c r="AO77" s="83">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="3:42" s="15" customFormat="1">
-      <c r="C78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="84"/>
-      <c r="F78" s="84"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="84"/>
-      <c r="I78" s="84"/>
+      <c r="C78" s="78"/>
+      <c r="D78" s="78"/>
+      <c r="E78" s="78"/>
+      <c r="F78" s="78"/>
+      <c r="G78" s="78"/>
+      <c r="H78" s="78"/>
+      <c r="I78" s="78"/>
       <c r="J78" s="78">
         <v>0</v>
       </c>
       <c r="K78" s="78" t="s">
-        <v>250</v>
-      </c>
-      <c r="L78" s="84"/>
-      <c r="M78" s="84"/>
-      <c r="N78" s="88"/>
-      <c r="O78" s="88"/>
-      <c r="P78" s="88"/>
-      <c r="Q78" s="88"/>
-      <c r="R78" s="88"/>
-      <c r="S78" s="88"/>
-      <c r="T78" s="88"/>
-      <c r="U78" s="88"/>
-      <c r="V78" s="88"/>
-      <c r="W78" s="88"/>
-      <c r="X78" s="88"/>
-      <c r="Y78" s="88"/>
-      <c r="Z78" s="88"/>
-      <c r="AA78" s="88"/>
-      <c r="AB78" s="88"/>
-      <c r="AC78" s="88"/>
-      <c r="AD78" s="88"/>
-      <c r="AE78" s="88"/>
-      <c r="AF78" s="88"/>
-      <c r="AG78" s="88"/>
-      <c r="AH78" s="88"/>
-      <c r="AI78" s="88"/>
-      <c r="AJ78" s="88"/>
-      <c r="AK78" s="88"/>
-      <c r="AL78" s="88"/>
-      <c r="AM78" s="88"/>
-      <c r="AN78" s="88"/>
-      <c r="AO78" s="91">
+        <v>122</v>
+      </c>
+      <c r="L78" s="78"/>
+      <c r="M78" s="78"/>
+      <c r="N78" s="89"/>
+      <c r="O78" s="89"/>
+      <c r="P78" s="89"/>
+      <c r="Q78" s="89"/>
+      <c r="R78" s="89"/>
+      <c r="S78" s="89"/>
+      <c r="T78" s="89"/>
+      <c r="U78" s="89"/>
+      <c r="V78" s="89"/>
+      <c r="W78" s="89"/>
+      <c r="X78" s="89"/>
+      <c r="Y78" s="89"/>
+      <c r="Z78" s="89"/>
+      <c r="AA78" s="89"/>
+      <c r="AB78" s="89"/>
+      <c r="AC78" s="89"/>
+      <c r="AD78" s="89"/>
+      <c r="AE78" s="89"/>
+      <c r="AF78" s="89"/>
+      <c r="AG78" s="89"/>
+      <c r="AH78" s="89"/>
+      <c r="AI78" s="89"/>
+      <c r="AJ78" s="89"/>
+      <c r="AK78" s="89"/>
+      <c r="AL78" s="89"/>
+      <c r="AM78" s="89"/>
+      <c r="AN78" s="89"/>
+      <c r="AO78" s="83">
         <v>5</v>
       </c>
     </row>
     <row r="79" spans="3:42" s="15" customFormat="1">
-      <c r="C79" s="84" t="s">
+      <c r="C79" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="D79" s="84"/>
-      <c r="E79" s="84" t="s">
-        <v>252</v>
-      </c>
-      <c r="F79" s="84"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="84" t="s">
-        <v>246</v>
-      </c>
-      <c r="I79" s="84"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="78" t="str">
+        <f>LEFT(C123,5)&amp;"*"</f>
+        <v>T-MGT*</v>
+      </c>
+      <c r="F79" s="78"/>
+      <c r="G79" s="78"/>
+      <c r="H79" s="78" t="str">
+        <f>H77</f>
+        <v>TRAF</v>
+      </c>
+      <c r="I79" s="78"/>
       <c r="J79" s="78">
         <v>2018</v>
       </c>
       <c r="K79" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="L79" s="84">
+        <v>122</v>
+      </c>
+      <c r="L79" s="78">
         <v>-1</v>
       </c>
-      <c r="M79" s="84" t="s">
+      <c r="M79" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="N79" s="88">
-        <f>ROUNDUP(C221,5)</f>
-        <v>9.8059999999999994E-2</v>
-      </c>
-      <c r="O79" s="88">
-        <f t="shared" ref="O79:AN79" si="28">ROUNDUP(D221,5)</f>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="P79" s="88">
+      <c r="N79" s="89">
+        <f>ROUNDDOWN(C221,5)</f>
+        <v>9.8049999999999998E-2</v>
+      </c>
+      <c r="O79" s="89">
+        <f t="shared" ref="O79:AN79" si="28">ROUNDDOWN(D221,5)</f>
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="P79" s="89">
         <f t="shared" si="28"/>
-        <v>9.774999999999999E-2</v>
-      </c>
-      <c r="Q79" s="88">
+        <v>9.7739999999999994E-2</v>
+      </c>
+      <c r="Q79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="R79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="R79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="S79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="S79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="T79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="T79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="U79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="U79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="V79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="V79" s="89">
         <f t="shared" si="28"/>
-        <v>9.663999999999999E-2</v>
-      </c>
-      <c r="W79" s="88">
+        <v>9.6629999999999994E-2</v>
+      </c>
+      <c r="W79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="X79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="X79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="Y79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="Y79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="Z79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="Z79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AA79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AA79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AB79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AB79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AC79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AC79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AD79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AD79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AE79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AE79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AF79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AF79" s="89">
         <f t="shared" si="28"/>
-        <v>9.4689999999999996E-2</v>
-      </c>
-      <c r="AG79" s="88">
+        <v>9.468E-2</v>
+      </c>
+      <c r="AG79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AH79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AH79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AI79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AI79" s="89">
         <f t="shared" si="28"/>
-        <v>8.8719999999999993E-2</v>
-      </c>
-      <c r="AJ79" s="88">
+        <v>8.8709999999999997E-2</v>
+      </c>
+      <c r="AJ79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AK79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AK79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AL79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AL79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AM79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AM79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AN79" s="88">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AN79" s="89">
         <f t="shared" si="28"/>
-        <v>9.8809999999999995E-2</v>
-      </c>
-      <c r="AO79" s="90">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="AO79" s="83">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="3:42" s="15" customFormat="1">
-      <c r="C80" s="84"/>
-      <c r="D80" s="84"/>
-      <c r="E80" s="84"/>
-      <c r="F80" s="84"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="84"/>
+      <c r="C80" s="78"/>
+      <c r="D80" s="78"/>
+      <c r="E80" s="78"/>
+      <c r="F80" s="78"/>
+      <c r="G80" s="78"/>
+      <c r="H80" s="78"/>
+      <c r="I80" s="78"/>
       <c r="J80" s="78">
         <v>0</v>
       </c>
       <c r="K80" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="L80" s="84"/>
-      <c r="M80" s="84"/>
-      <c r="N80" s="88"/>
-      <c r="O80" s="88"/>
-      <c r="P80" s="88"/>
-      <c r="Q80" s="88"/>
-      <c r="R80" s="88"/>
-      <c r="S80" s="88"/>
-      <c r="T80" s="88"/>
-      <c r="U80" s="88"/>
-      <c r="V80" s="88"/>
-      <c r="W80" s="88"/>
-      <c r="X80" s="88"/>
-      <c r="Y80" s="88"/>
-      <c r="Z80" s="88"/>
-      <c r="AA80" s="88"/>
-      <c r="AB80" s="88"/>
-      <c r="AC80" s="88"/>
-      <c r="AD80" s="88"/>
-      <c r="AE80" s="88"/>
-      <c r="AF80" s="88"/>
-      <c r="AG80" s="88"/>
-      <c r="AH80" s="88"/>
-      <c r="AI80" s="88"/>
-      <c r="AJ80" s="88"/>
-      <c r="AK80" s="88"/>
-      <c r="AL80" s="88"/>
-      <c r="AM80" s="88"/>
-      <c r="AN80" s="88"/>
-      <c r="AO80" s="91">
+        <v>122</v>
+      </c>
+      <c r="L80" s="78"/>
+      <c r="M80" s="78"/>
+      <c r="N80" s="89"/>
+      <c r="O80" s="89"/>
+      <c r="P80" s="89"/>
+      <c r="Q80" s="89"/>
+      <c r="R80" s="89"/>
+      <c r="S80" s="89"/>
+      <c r="T80" s="89"/>
+      <c r="U80" s="89"/>
+      <c r="V80" s="89"/>
+      <c r="W80" s="89"/>
+      <c r="X80" s="89"/>
+      <c r="Y80" s="89"/>
+      <c r="Z80" s="89"/>
+      <c r="AA80" s="89"/>
+      <c r="AB80" s="89"/>
+      <c r="AC80" s="89"/>
+      <c r="AD80" s="89"/>
+      <c r="AE80" s="89"/>
+      <c r="AF80" s="89"/>
+      <c r="AG80" s="89"/>
+      <c r="AH80" s="89"/>
+      <c r="AI80" s="89"/>
+      <c r="AJ80" s="89"/>
+      <c r="AK80" s="89"/>
+      <c r="AL80" s="89"/>
+      <c r="AM80" s="89"/>
+      <c r="AN80" s="89"/>
+      <c r="AO80" s="83">
         <v>5</v>
       </c>
     </row>
     <row r="81" spans="3:41" s="15" customFormat="1">
-      <c r="C81" s="84" t="s">
+      <c r="C81" s="78" t="s">
         <v>242</v>
       </c>
-      <c r="D81" s="84"/>
-      <c r="E81" s="84" t="s">
-        <v>253</v>
-      </c>
-      <c r="F81" s="84"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="84" t="s">
-        <v>246</v>
-      </c>
-      <c r="I81" s="84"/>
+      <c r="D81" s="78"/>
+      <c r="E81" s="78" t="str">
+        <f>LEFT(C124,5)&amp;"*"</f>
+        <v>T-HGT*</v>
+      </c>
+      <c r="F81" s="78"/>
+      <c r="G81" s="78"/>
+      <c r="H81" s="78" t="str">
+        <f>H79</f>
+        <v>TRAF</v>
+      </c>
+      <c r="I81" s="78"/>
       <c r="J81" s="78">
         <v>2018</v>
       </c>
       <c r="K81" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="L81" s="84">
+        <v>122</v>
+      </c>
+      <c r="L81" s="78">
         <v>-1</v>
       </c>
-      <c r="M81" s="84" t="s">
+      <c r="M81" s="78" t="s">
         <v>243</v>
       </c>
-      <c r="N81" s="88">
-        <f>ROUNDUP(C222,5)</f>
-        <v>0.86921999999999999</v>
-      </c>
-      <c r="O81" s="88">
-        <f t="shared" ref="O81:AN81" si="29">ROUNDUP(D222,5)</f>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="P81" s="88">
+      <c r="N81" s="89">
+        <f>ROUNDDOWN(C222,5)</f>
+        <v>0.86921000000000004</v>
+      </c>
+      <c r="O81" s="89">
+        <f t="shared" ref="O81:AN81" si="29">ROUNDDOWN(D222,5)</f>
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="P81" s="89">
         <f t="shared" si="29"/>
-        <v>0.86651</v>
-      </c>
-      <c r="Q81" s="88">
+        <v>0.86650000000000005</v>
+      </c>
+      <c r="Q81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="R81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="R81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="S81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="S81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="T81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="T81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="U81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="U81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="V81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="V81" s="89">
         <f t="shared" si="29"/>
-        <v>0.85666999999999993</v>
-      </c>
-      <c r="W81" s="88">
+        <v>0.85665999999999998</v>
+      </c>
+      <c r="W81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="X81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="X81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="Y81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="Y81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="Z81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="Z81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AA81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AA81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AB81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AB81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AC81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AC81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AD81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AD81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AE81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AE81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AF81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AF81" s="89">
         <f t="shared" si="29"/>
-        <v>0.83933999999999997</v>
-      </c>
-      <c r="AG81" s="88">
+        <v>0.83933000000000002</v>
+      </c>
+      <c r="AG81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AH81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AH81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AI81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AI81" s="89">
         <f t="shared" si="29"/>
-        <v>0.78648999999999991</v>
-      </c>
-      <c r="AJ81" s="88">
+        <v>0.78647999999999996</v>
+      </c>
+      <c r="AJ81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AK81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AK81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AL81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AL81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AM81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AM81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AN81" s="88">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AN81" s="89">
         <f t="shared" si="29"/>
-        <v>0.87588999999999995</v>
-      </c>
-      <c r="AO81" s="90">
+        <v>0.87587999999999999</v>
+      </c>
+      <c r="AO81" s="83">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="3:41" s="15" customFormat="1">
-      <c r="C82" s="84"/>
-      <c r="D82" s="84"/>
-      <c r="E82" s="84"/>
-      <c r="F82" s="84"/>
-      <c r="G82" s="84"/>
-      <c r="H82" s="84"/>
-      <c r="I82" s="84"/>
-      <c r="J82" s="84">
-        <v>0</v>
-      </c>
-      <c r="K82" s="84" t="s">
-        <v>66</v>
-      </c>
-      <c r="L82" s="84"/>
-      <c r="M82" s="84"/>
-      <c r="N82" s="89"/>
-      <c r="O82" s="89"/>
-      <c r="P82" s="89"/>
-      <c r="Q82" s="89"/>
-      <c r="R82" s="89"/>
-      <c r="S82" s="89"/>
-      <c r="T82" s="89"/>
-      <c r="U82" s="89"/>
-      <c r="V82" s="89"/>
-      <c r="W82" s="89"/>
-      <c r="X82" s="89"/>
-      <c r="Y82" s="89"/>
-      <c r="Z82" s="89"/>
-      <c r="AA82" s="89"/>
-      <c r="AB82" s="89"/>
-      <c r="AC82" s="89"/>
-      <c r="AD82" s="89"/>
-      <c r="AE82" s="89"/>
-      <c r="AF82" s="89"/>
-      <c r="AG82" s="89"/>
-      <c r="AH82" s="89"/>
-      <c r="AI82" s="89"/>
-      <c r="AJ82" s="89"/>
-      <c r="AK82" s="89"/>
-      <c r="AL82" s="89"/>
-      <c r="AM82" s="89"/>
-      <c r="AN82" s="89"/>
-      <c r="AO82" s="84">
+      <c r="C82" s="78"/>
+      <c r="D82" s="78"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="78"/>
+      <c r="G82" s="78"/>
+      <c r="H82" s="78"/>
+      <c r="I82" s="78"/>
+      <c r="J82" s="78">
+        <v>0</v>
+      </c>
+      <c r="K82" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="L82" s="78"/>
+      <c r="M82" s="78"/>
+      <c r="N82" s="82"/>
+      <c r="O82" s="82"/>
+      <c r="P82" s="82"/>
+      <c r="Q82" s="82"/>
+      <c r="R82" s="82"/>
+      <c r="S82" s="82"/>
+      <c r="T82" s="82"/>
+      <c r="U82" s="82"/>
+      <c r="V82" s="82"/>
+      <c r="W82" s="82"/>
+      <c r="X82" s="82"/>
+      <c r="Y82" s="82"/>
+      <c r="Z82" s="82"/>
+      <c r="AA82" s="82"/>
+      <c r="AB82" s="82"/>
+      <c r="AC82" s="82"/>
+      <c r="AD82" s="82"/>
+      <c r="AE82" s="82"/>
+      <c r="AF82" s="82"/>
+      <c r="AG82" s="82"/>
+      <c r="AH82" s="82"/>
+      <c r="AI82" s="82"/>
+      <c r="AJ82" s="82"/>
+      <c r="AK82" s="82"/>
+      <c r="AL82" s="82"/>
+      <c r="AM82" s="82"/>
+      <c r="AN82" s="82"/>
+      <c r="AO82" s="78">
         <v>5</v>
       </c>
     </row>
     <row r="83" spans="3:41" s="15" customFormat="1">
-      <c r="C83" s="84" t="s">
+      <c r="C83" s="78" t="s">
         <v>244</v>
       </c>
-      <c r="D83" s="84"/>
-      <c r="E83" s="84" t="s">
-        <v>254</v>
-      </c>
-      <c r="F83" s="84"/>
-      <c r="G83" s="84"/>
-      <c r="H83" s="84" t="s">
+      <c r="D83" s="78"/>
+      <c r="E83" s="78" t="s">
+        <v>250</v>
+      </c>
+      <c r="F83" s="78"/>
+      <c r="G83" s="78"/>
+      <c r="H83" s="78" t="s">
         <v>246</v>
       </c>
-      <c r="I83" s="84"/>
-      <c r="J83" s="86">
+      <c r="I83" s="78"/>
+      <c r="J83" s="78">
         <v>2018</v>
       </c>
-      <c r="K83" s="86" t="s">
-        <v>66</v>
-      </c>
-      <c r="L83" s="84">
+      <c r="K83" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="L83" s="78">
         <v>-1</v>
       </c>
-      <c r="M83" s="84" t="s">
+      <c r="M83" s="78" t="s">
         <v>245</v>
       </c>
-      <c r="N83" s="88">
-        <f>ROUNDUP(C223,5)</f>
-        <v>7.6199999999999992E-3</v>
-      </c>
-      <c r="O83" s="88">
-        <f t="shared" ref="O83:AN83" si="30">ROUNDUP(D223,5)</f>
-        <v>0</v>
-      </c>
-      <c r="P83" s="88">
+      <c r="N83" s="89">
+        <f>ROUNDDOWN(C223,5)</f>
+        <v>7.6099999999999996E-3</v>
+      </c>
+      <c r="O83" s="89">
+        <f t="shared" ref="O83:AN83" si="30">ROUNDDOWN(D223,5)</f>
+        <v>0</v>
+      </c>
+      <c r="P83" s="89">
         <f t="shared" si="30"/>
-        <v>1.0709999999999999E-2</v>
-      </c>
-      <c r="Q83" s="88">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="Q83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="R83" s="88">
+      <c r="R83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="S83" s="88">
+      <c r="S83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="T83" s="88">
+      <c r="T83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="U83" s="88">
+      <c r="U83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="V83" s="88">
+      <c r="V83" s="89">
         <f t="shared" si="30"/>
-        <v>2.1950000000000001E-2</v>
-      </c>
-      <c r="W83" s="88">
+        <v>2.1940000000000001E-2</v>
+      </c>
+      <c r="W83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="X83" s="88">
+      <c r="X83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="Y83" s="88">
+      <c r="Y83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="Z83" s="88">
+      <c r="Z83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AA83" s="88">
+      <c r="AA83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AB83" s="88">
+      <c r="AB83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AC83" s="88">
+      <c r="AC83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AD83" s="88">
+      <c r="AD83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AE83" s="88">
+      <c r="AE83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AF83" s="88">
+      <c r="AF83" s="89">
         <f t="shared" si="30"/>
-        <v>4.1730000000000003E-2</v>
-      </c>
-      <c r="AG83" s="88">
+        <v>4.172E-2</v>
+      </c>
+      <c r="AG83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AH83" s="88">
+      <c r="AH83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AI83" s="88">
+      <c r="AI83" s="89">
         <f t="shared" si="30"/>
-        <v>0.10207999999999999</v>
-      </c>
-      <c r="AJ83" s="88">
+        <v>0.10206999999999999</v>
+      </c>
+      <c r="AJ83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AK83" s="88">
+      <c r="AK83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AL83" s="88">
+      <c r="AL83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AM83" s="88">
+      <c r="AM83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AN83" s="88">
+      <c r="AN83" s="89">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AO83" s="90">
+      <c r="AO83" s="83">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="3:41" s="15" customFormat="1">
-      <c r="C84" s="83"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="83"/>
-      <c r="F84" s="83"/>
-      <c r="G84" s="83"/>
-      <c r="H84" s="83"/>
-      <c r="I84" s="83"/>
-      <c r="J84" s="85">
-        <v>0</v>
-      </c>
-      <c r="K84" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="L84" s="83"/>
-      <c r="M84" s="83"/>
-      <c r="N84" s="83"/>
-      <c r="O84" s="83"/>
-      <c r="P84" s="83"/>
-      <c r="Q84" s="83"/>
-      <c r="R84" s="83"/>
-      <c r="S84" s="83"/>
-      <c r="T84" s="83"/>
-      <c r="U84" s="83"/>
-      <c r="V84" s="83"/>
-      <c r="W84" s="83"/>
-      <c r="X84" s="83"/>
-      <c r="Y84" s="83"/>
-      <c r="Z84" s="83"/>
-      <c r="AA84" s="83"/>
-      <c r="AB84" s="83"/>
-      <c r="AC84" s="83"/>
-      <c r="AD84" s="83"/>
-      <c r="AE84" s="83"/>
-      <c r="AF84" s="83"/>
-      <c r="AG84" s="83"/>
-      <c r="AH84" s="83"/>
-      <c r="AI84" s="83"/>
-      <c r="AJ84" s="83"/>
-      <c r="AK84" s="83"/>
-      <c r="AL84" s="83"/>
-      <c r="AM84" s="83"/>
-      <c r="AN84" s="83"/>
-      <c r="AO84" s="83">
+      <c r="C84" s="80"/>
+      <c r="D84" s="80"/>
+      <c r="E84" s="80"/>
+      <c r="F84" s="80"/>
+      <c r="G84" s="80"/>
+      <c r="H84" s="80"/>
+      <c r="I84" s="80"/>
+      <c r="J84" s="80">
+        <v>0</v>
+      </c>
+      <c r="K84" s="80" t="s">
+        <v>122</v>
+      </c>
+      <c r="L84" s="80"/>
+      <c r="M84" s="80"/>
+      <c r="N84" s="80"/>
+      <c r="O84" s="80"/>
+      <c r="P84" s="80"/>
+      <c r="Q84" s="80"/>
+      <c r="R84" s="80"/>
+      <c r="S84" s="80"/>
+      <c r="T84" s="80"/>
+      <c r="U84" s="80"/>
+      <c r="V84" s="80"/>
+      <c r="W84" s="80"/>
+      <c r="X84" s="80"/>
+      <c r="Y84" s="80"/>
+      <c r="Z84" s="80"/>
+      <c r="AA84" s="80"/>
+      <c r="AB84" s="80"/>
+      <c r="AC84" s="80"/>
+      <c r="AD84" s="80"/>
+      <c r="AE84" s="80"/>
+      <c r="AF84" s="80"/>
+      <c r="AG84" s="80"/>
+      <c r="AH84" s="80"/>
+      <c r="AI84" s="80"/>
+      <c r="AJ84" s="80"/>
+      <c r="AK84" s="80"/>
+      <c r="AL84" s="80"/>
+      <c r="AM84" s="80"/>
+      <c r="AN84" s="80"/>
+      <c r="AO84" s="80">
         <v>5</v>
       </c>
     </row>
     <row r="85" spans="3:41" s="15" customFormat="1">
-      <c r="C85" s="84"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="84"/>
-      <c r="I85" s="84"/>
-      <c r="J85" s="84"/>
-      <c r="K85" s="84"/>
-      <c r="L85" s="84"/>
-      <c r="M85" s="84"/>
-      <c r="N85" s="84"/>
-      <c r="O85" s="84"/>
-      <c r="P85" s="84"/>
-      <c r="Q85" s="84"/>
-      <c r="R85" s="84"/>
-      <c r="S85" s="84"/>
-      <c r="T85" s="84"/>
-      <c r="U85" s="84"/>
-      <c r="V85" s="84"/>
-      <c r="W85" s="84"/>
-      <c r="X85" s="84"/>
-      <c r="Y85" s="84"/>
-      <c r="Z85" s="84"/>
-      <c r="AA85" s="84"/>
-      <c r="AB85" s="84"/>
-      <c r="AC85" s="84"/>
-      <c r="AD85" s="84"/>
-      <c r="AE85" s="84"/>
-      <c r="AF85" s="84"/>
-      <c r="AG85" s="84"/>
-      <c r="AH85" s="84"/>
-      <c r="AI85" s="84"/>
-      <c r="AJ85" s="84"/>
-      <c r="AK85" s="84"/>
-      <c r="AL85" s="84"/>
-      <c r="AM85" s="84"/>
-      <c r="AN85" s="84"/>
-      <c r="AO85" s="84"/>
+      <c r="C85" s="78"/>
+      <c r="D85" s="78"/>
+      <c r="E85" s="78"/>
+      <c r="F85" s="78"/>
+      <c r="G85" s="78"/>
+      <c r="H85" s="78"/>
+      <c r="I85" s="78"/>
+      <c r="J85" s="78"/>
+      <c r="K85" s="78"/>
+      <c r="L85" s="78"/>
+      <c r="M85" s="78"/>
+      <c r="N85" s="78"/>
+      <c r="O85" s="78"/>
+      <c r="P85" s="78"/>
+      <c r="Q85" s="78"/>
+      <c r="R85" s="78"/>
+      <c r="S85" s="78"/>
+      <c r="T85" s="78"/>
+      <c r="U85" s="78"/>
+      <c r="V85" s="78"/>
+      <c r="W85" s="78"/>
+      <c r="X85" s="78"/>
+      <c r="Y85" s="78"/>
+      <c r="Z85" s="78"/>
+      <c r="AA85" s="78"/>
+      <c r="AB85" s="78"/>
+      <c r="AC85" s="78"/>
+      <c r="AD85" s="78"/>
+      <c r="AE85" s="78"/>
+      <c r="AF85" s="78"/>
+      <c r="AG85" s="78"/>
+      <c r="AH85" s="78"/>
+      <c r="AI85" s="78"/>
+      <c r="AJ85" s="78"/>
+      <c r="AK85" s="78"/>
+      <c r="AL85" s="78"/>
+      <c r="AM85" s="78"/>
+      <c r="AN85" s="78"/>
+      <c r="AO85" s="78"/>
     </row>
     <row r="86" spans="3:41" s="15" customFormat="1">
-      <c r="C86" s="84"/>
-      <c r="D86" s="84"/>
-      <c r="E86" s="84"/>
-      <c r="F86" s="84"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
-      <c r="J86" s="86"/>
-      <c r="K86" s="84"/>
-      <c r="L86" s="84"/>
+      <c r="C86" s="78"/>
+      <c r="D86" s="78"/>
+      <c r="E86" s="78"/>
+      <c r="F86" s="78"/>
+      <c r="G86" s="78"/>
+      <c r="H86" s="78"/>
+      <c r="I86" s="78"/>
+      <c r="J86" s="78"/>
+      <c r="K86" s="78"/>
+      <c r="L86" s="78"/>
       <c r="M86" s="78" t="s">
         <v>220</v>
       </c>
-      <c r="N86" s="92">
-        <v>1</v>
-      </c>
-      <c r="O86" s="87">
-        <v>1</v>
-      </c>
-      <c r="P86" s="87">
-        <v>0.99999000000000005</v>
-      </c>
-      <c r="Q86" s="87">
-        <v>1</v>
-      </c>
-      <c r="R86" s="87">
-        <v>1</v>
-      </c>
-      <c r="S86" s="87">
-        <v>1</v>
-      </c>
-      <c r="T86" s="87">
-        <v>1</v>
-      </c>
-      <c r="U86" s="87">
-        <v>1</v>
-      </c>
-      <c r="V86" s="87">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="W86" s="87">
-        <v>1</v>
-      </c>
-      <c r="X86" s="87">
-        <v>1</v>
-      </c>
-      <c r="Y86" s="87">
-        <v>1</v>
-      </c>
-      <c r="Z86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AA86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AB86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AC86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AD86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AE86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AF86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AG86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AH86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AI86" s="87">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="AJ86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AK86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AL86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AM86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AN86" s="87">
-        <v>1</v>
-      </c>
-      <c r="AO86" s="84"/>
+      <c r="N86" s="84">
+        <f>N77+N79+N81+N83</f>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="O86" s="84">
+        <f t="shared" ref="O86:AN86" si="31">O77+O79+O81+O83</f>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="P86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997000000000014</v>
+      </c>
+      <c r="Q86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="R86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="S86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="T86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="U86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="V86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="W86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="X86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="Y86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="Z86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AA86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AB86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AC86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AD86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AE86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AF86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AG86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AH86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AI86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AJ86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AK86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AL86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AM86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AN86" s="82">
+        <f t="shared" si="31"/>
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="AO86" s="78"/>
     </row>
     <row r="87" spans="3:41" s="15" customFormat="1">
       <c r="N87" s="60"/>
@@ -13689,107 +13729,107 @@
         <v>11626.550999999999</v>
       </c>
       <c r="D205" s="66">
-        <f t="shared" ref="D205:AC205" si="31">SUM(D201:D204)</f>
+        <f t="shared" ref="D205:AC205" si="32">SUM(D201:D204)</f>
         <v>177.95641949867974</v>
       </c>
       <c r="E205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2657.9186883230773</v>
       </c>
       <c r="F205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>482.32584543324703</v>
       </c>
       <c r="G205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>310.17655131899437</v>
       </c>
       <c r="H205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>220.92382768752688</v>
       </c>
       <c r="I205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>106.61321663190297</v>
       </c>
       <c r="J205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>279.38412011837357</v>
       </c>
       <c r="K205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>432.28792622333316</v>
       </c>
       <c r="L205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>203.35363153768466</v>
       </c>
       <c r="M205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>231.54784920152733</v>
       </c>
       <c r="N205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>467.99675121515725</v>
       </c>
       <c r="O205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>308.73718466108562</v>
       </c>
       <c r="P205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>303.81359843254126</v>
       </c>
       <c r="Q205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1625.5685935130527</v>
       </c>
       <c r="R205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>442.29510717528478</v>
       </c>
       <c r="S205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>498.35433078518957</v>
       </c>
       <c r="T205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>407.97504625354344</v>
       </c>
       <c r="U205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>378.95230113305684</v>
       </c>
       <c r="V205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>605.11341326480942</v>
       </c>
       <c r="W205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>80.700464509738026</v>
       </c>
       <c r="X205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>340.81032279518195</v>
       </c>
       <c r="Y205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>151.34752708989396</v>
       </c>
       <c r="Z205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>165.04509242434406</v>
       </c>
       <c r="AA205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>191.84367071819389</v>
       </c>
       <c r="AB205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>400.91337992242592</v>
       </c>
       <c r="AC205" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>154.59614013215509</v>
       </c>
     </row>
@@ -13927,107 +13967,107 @@
         <v>2.5114928752301521E-2</v>
       </c>
       <c r="D220" s="72">
-        <f t="shared" ref="D220:AC220" si="32">D201/D205</f>
+        <f t="shared" ref="D220:AC220" si="33">D201/D205</f>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="E220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5036666940775776E-2</v>
       </c>
       <c r="F220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="G220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="H220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="I220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="J220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="K220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.475224056984587E-2</v>
       </c>
       <c r="L220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="M220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="N220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="O220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="P220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="Q220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825624E-2</v>
       </c>
       <c r="R220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="S220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="T220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="U220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.4251656377299691E-2</v>
       </c>
       <c r="V220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="W220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825624E-2</v>
       </c>
       <c r="X220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.2724421467469183E-2</v>
       </c>
       <c r="Y220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="Z220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
       <c r="AA220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825614E-2</v>
       </c>
       <c r="AB220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825617E-2</v>
       </c>
       <c r="AC220" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.5307678973825621E-2</v>
       </c>
     </row>
@@ -14043,107 +14083,107 @@
         <v>9.8051434169944301E-2</v>
       </c>
       <c r="D221" s="72">
-        <f t="shared" ref="D221:AC221" si="33">D202/D205</f>
+        <f t="shared" ref="D221:AC221" si="34">D202/D205</f>
         <v>9.8803952158086308E-2</v>
       </c>
       <c r="E221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.7745891481110916E-2</v>
       </c>
       <c r="F221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="G221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="H221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="I221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="J221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="K221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.663545975898731E-2</v>
       </c>
       <c r="L221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="M221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="N221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="O221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="P221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="Q221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
       <c r="R221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="S221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
       <c r="T221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="U221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.4681124212745368E-2</v>
       </c>
       <c r="V221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="W221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
       <c r="X221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8718631756557781E-2</v>
       </c>
       <c r="Y221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086336E-2</v>
       </c>
       <c r="Z221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
       <c r="AA221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086308E-2</v>
       </c>
       <c r="AB221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086308E-2</v>
       </c>
       <c r="AC221" s="72">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>9.8803952158086322E-2</v>
       </c>
     </row>
@@ -14159,27 +14199,27 @@
         <v>0.86921736291355889</v>
       </c>
       <c r="D222" s="72">
-        <f t="shared" ref="D222:AC222" si="34">D203/D205</f>
+        <f t="shared" ref="D222:AC222" si="35">D203/D205</f>
         <v>0.87588836886808807</v>
       </c>
       <c r="E222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.86650875377904113</v>
       </c>
       <c r="F222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="G222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="H222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="I222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="J222" s="72">
@@ -14187,79 +14227,79 @@
         <v>0.87588836886808807</v>
       </c>
       <c r="K222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.85666487396870683</v>
       </c>
       <c r="L222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="M222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
       <c r="N222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="O222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
       <c r="P222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="Q222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="R222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="S222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="T222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
       <c r="U222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.83933986078421474</v>
       </c>
       <c r="V222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="W222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="X222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.78648288818576562</v>
       </c>
       <c r="Y222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808819</v>
       </c>
       <c r="Z222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="AA222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808796</v>
       </c>
       <c r="AB222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808807</v>
       </c>
       <c r="AC222" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.87588836886808819</v>
       </c>
     </row>
@@ -14275,107 +14315,107 @@
         <v>7.616274164195384E-3</v>
       </c>
       <c r="D223" s="72">
-        <f t="shared" ref="D223:AC223" si="35">D204/D205</f>
+        <f t="shared" ref="D223:AC223" si="36">D204/D205</f>
         <v>0</v>
       </c>
       <c r="E223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.070868779907224E-2</v>
       </c>
       <c r="F223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="H223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="K223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>2.1947425702460069E-2</v>
       </c>
       <c r="L223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="P223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Q223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="R223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="S223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="U223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>4.1727358625740237E-2</v>
       </c>
       <c r="V223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="X223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.10207405859020728</v>
       </c>
       <c r="Y223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AA223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AB223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AC223" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -14389,107 +14429,107 @@
         <v>1</v>
       </c>
       <c r="D224" s="74">
-        <f t="shared" ref="D224:AC224" si="36">SUM(D220:D223)</f>
+        <f t="shared" ref="D224:AC224" si="37">SUM(D220:D223)</f>
         <v>1</v>
       </c>
       <c r="E224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="F224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="G224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="H224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="I224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="J224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="K224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="L224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="M224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="N224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="O224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="P224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="Q224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="R224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="S224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="T224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="U224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="V224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="W224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="X224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="Y224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="Z224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="AA224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="AB224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="AC224" s="74">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1.0000000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update with shares from VT to resolve a dummies
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_ActiveModes.xlsx
+++ b/SuppXLS/Scen_TRA_ActiveModes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5B0396-CD0B-4C84-A5FA-EE50F27655F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AD136C-73CB-44B5-B909-85B3F25ECA98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -745,6 +745,7 @@
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1093,7 +1094,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1195,6 +1196,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="171" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="20% - Accent5 2" xfId="9" xr:uid="{7F8DC7F5-A9E6-4E53-9FB8-C5D57F662307}"/>
@@ -2383,8 +2385,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:AQ177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2941,7 +2943,7 @@
       </c>
       <c r="AH12" s="52">
         <f t="shared" si="0"/>
-        <v>0.30599999999999999</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="AI12" s="52">
         <f t="shared" si="0"/>
@@ -3080,7 +3082,7 @@
       </c>
       <c r="AH13" s="10">
         <f t="shared" si="1"/>
-        <v>0.497989762973442</v>
+        <v>0.496362345447385</v>
       </c>
       <c r="AI13" s="10">
         <f t="shared" si="1"/>
@@ -3601,7 +3603,7 @@
       </c>
       <c r="AH18" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AI18" s="10">
         <f t="shared" si="4"/>
@@ -3740,7 +3742,7 @@
       </c>
       <c r="AH19" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AI19" s="10">
         <f t="shared" si="5"/>
@@ -3931,7 +3933,7 @@
       </c>
       <c r="AH21" s="52">
         <f t="shared" si="6"/>
-        <v>0.57199999999999995</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="AI21" s="52">
         <f t="shared" si="6"/>
@@ -4070,7 +4072,7 @@
       </c>
       <c r="AH22" s="10">
         <f t="shared" si="7"/>
-        <v>0.28599999999999998</v>
+        <v>0.28549999999999998</v>
       </c>
       <c r="AI22" s="10">
         <f t="shared" si="7"/>
@@ -5279,7 +5281,7 @@
       </c>
       <c r="AH34" s="50">
         <f t="shared" si="14"/>
-        <v>1.0029999999999999</v>
+        <v>1.0025999999999999</v>
       </c>
       <c r="AI34" s="50">
         <f t="shared" si="14"/>
@@ -5405,7 +5407,7 @@
       </c>
       <c r="AH35" s="50">
         <f t="shared" si="14"/>
-        <v>0.95998976297344196</v>
+        <v>0.95946234544738496</v>
       </c>
       <c r="AI35" s="50">
         <f t="shared" si="14"/>
@@ -5709,7 +5711,7 @@
       </c>
       <c r="P41" s="50">
         <f t="shared" si="16"/>
-        <v>4.4000000000000003E-3</v>
+        <v>4.2000000000000006E-3</v>
       </c>
       <c r="Q41" s="50">
         <f t="shared" si="16"/>
@@ -5781,7 +5783,7 @@
       </c>
       <c r="AH41" s="50">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="AI41" s="50">
         <f t="shared" si="16"/>
@@ -5956,7 +5958,7 @@
       </c>
       <c r="AH43" s="52">
         <f t="shared" si="17"/>
-        <v>0.89</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="AI43" s="52">
         <f t="shared" si="17"/>
@@ -6306,7 +6308,7 @@
       </c>
       <c r="AH47" s="10">
         <f t="shared" si="19"/>
-        <v>0.11</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="AI47" s="10">
         <f t="shared" si="19"/>
@@ -6576,7 +6578,7 @@
       </c>
       <c r="P52" s="50">
         <f t="shared" si="21"/>
-        <v>1.0064</v>
+        <v>1.0062</v>
       </c>
       <c r="Q52" s="50">
         <f t="shared" si="21"/>
@@ -6648,7 +6650,7 @@
       </c>
       <c r="AH52" s="50">
         <f t="shared" si="21"/>
-        <v>1.0110000000000001</v>
+        <v>1.0011000000000001</v>
       </c>
       <c r="AI52" s="50">
         <f t="shared" si="21"/>
@@ -8486,7 +8488,7 @@
         <v>0.29539615700051852</v>
       </c>
       <c r="E141" s="44">
-        <v>0.34966256439645477</v>
+        <v>0.34967728765163869</v>
       </c>
       <c r="F141" s="44">
         <v>0.31311359703458036</v>
@@ -8540,7 +8542,7 @@
         <v>0.31520515014132622</v>
       </c>
       <c r="W141" s="44">
-        <v>0.30543827437637427</v>
+        <v>0.30496664626628506</v>
       </c>
       <c r="X141" s="44">
         <v>0.29765342162432462</v>
@@ -8566,14 +8568,14 @@
       <c r="B142" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="C142" s="44">
+      <c r="C142" s="57">
         <v>5.3963306308090382E-2</v>
       </c>
       <c r="D142" s="44">
         <v>4.9232692833419758E-2</v>
       </c>
       <c r="E142" s="44">
-        <v>5.8277094066075792E-2</v>
+        <v>5.8279547941939784E-2</v>
       </c>
       <c r="F142" s="44">
         <v>5.2185599505763403E-2</v>
@@ -8627,7 +8629,7 @@
         <v>5.2534191690221041E-2</v>
       </c>
       <c r="W142" s="44">
-        <v>5.0906379062729046E-2</v>
+        <v>5.0827774377714179E-2</v>
       </c>
       <c r="X142" s="44">
         <v>4.9608903604054101E-2</v>
@@ -8662,7 +8664,7 @@
         <v>8.4181954391599476E-4</v>
       </c>
       <c r="E143" s="44">
-        <v>1.4736843073167786E-3</v>
+        <v>1.4316393209477573E-3</v>
       </c>
       <c r="F143" s="44">
         <v>1.3698908311171865E-3</v>
@@ -8716,7 +8718,7 @@
         <v>7.9269582890742734E-4</v>
       </c>
       <c r="W143" s="44">
-        <v>0</v>
+        <v>1.544102850410962E-3</v>
       </c>
       <c r="X143" s="44">
         <v>7.4007830335184128E-4</v>
@@ -8749,7 +8751,7 @@
         <v>0.57696936147650701</v>
       </c>
       <c r="E144" s="44">
-        <v>0.41519891685215071</v>
+        <v>0.4152163996490737</v>
       </c>
       <c r="F144" s="44">
         <v>0.53837411623785481</v>
@@ -8803,7 +8805,7 @@
         <v>0.5314898835087899</v>
       </c>
       <c r="W144" s="44">
-        <v>0.5710449216561202</v>
+        <v>0.57016316956487822</v>
       </c>
       <c r="X144" s="44">
         <v>0.54463316447281129</v>
@@ -8838,7 +8840,7 @@
         <v>7.4490307781118984E-3</v>
       </c>
       <c r="E145" s="44">
-        <v>3.2041705931306341E-2</v>
+        <v>3.2043055112662859E-2</v>
       </c>
       <c r="F145" s="44">
         <v>1.4142087272297982E-2</v>
@@ -8892,7 +8894,7 @@
         <v>1.3327262086971724E-2</v>
       </c>
       <c r="W145" s="44">
-        <v>8.2106842864435349E-3</v>
+        <v>8.1980061454330136E-3</v>
       </c>
       <c r="X145" s="44">
         <v>7.2036254203120672E-3</v>
@@ -8925,7 +8927,7 @@
         <v>7.0110938367526743E-2</v>
       </c>
       <c r="E146" s="44">
-        <v>0.1139689510378053</v>
+        <v>0.11397374993285452</v>
       </c>
       <c r="F146" s="44">
         <v>8.0814709118386313E-2</v>
@@ -8979,7 +8981,7 @@
         <v>8.6650816743783748E-2</v>
       </c>
       <c r="W146" s="44">
-        <v>6.4399740618333048E-2</v>
+        <v>6.4300300795278542E-2</v>
       </c>
       <c r="X146" s="44">
         <v>0.10016080657514609</v>
@@ -9012,7 +9014,7 @@
         <v>0</v>
       </c>
       <c r="E147" s="44">
-        <v>2.9377083408890298E-2</v>
+        <v>2.9378320390882739E-2</v>
       </c>
       <c r="F147" s="44">
         <v>0</v>
@@ -9666,7 +9668,7 @@
         <v>2.1586268841599747E-3</v>
       </c>
       <c r="E157" s="44">
-        <v>4.3137182635283444E-3</v>
+        <v>4.1909857054726746E-3</v>
       </c>
       <c r="F157" s="44">
         <v>3.6319751739066989E-3</v>
@@ -9720,7 +9722,7 @@
         <v>2.1106258862285242E-3</v>
       </c>
       <c r="W157" s="44">
-        <v>0</v>
+        <v>4.0260002016890241E-3</v>
       </c>
       <c r="X157" s="44">
         <v>1.9054783663146626E-3</v>
@@ -9753,7 +9755,7 @@
         <v>0.88136996225712338</v>
       </c>
       <c r="E158" s="44">
-        <v>0.7240198055510555</v>
+        <v>0.72410905133504211</v>
       </c>
       <c r="F158" s="44">
         <v>0.85033097733510543</v>
@@ -9807,7 +9809,7 @@
         <v>0.84303694258501916</v>
       </c>
       <c r="W158" s="44">
-        <v>0.88919219682824724</v>
+        <v>0.88561230886447639</v>
       </c>
       <c r="X158" s="44">
         <v>0.83536706688667051</v>
@@ -9842,7 +9844,7 @@
         <v>9.3709663140288998E-3</v>
       </c>
       <c r="E159" s="44">
-        <v>4.6013893098741668E-2</v>
+        <v>4.6019564968395495E-2</v>
       </c>
       <c r="F159" s="44">
         <v>1.8394858695029128E-2</v>
@@ -9896,7 +9898,7 @@
         <v>1.7408913059663488E-2</v>
       </c>
       <c r="W159" s="44">
-        <v>1.0528920260910977E-2</v>
+        <v>1.0486530825816983E-2</v>
       </c>
       <c r="X159" s="44">
         <v>9.0992061135074936E-3</v>
@@ -9929,7 +9931,7 @@
         <v>0.10710044454468777</v>
       </c>
       <c r="E160" s="44">
-        <v>0.19873794082808949</v>
+        <v>0.19876243811835848</v>
       </c>
       <c r="F160" s="44">
         <v>0.12764218879595873</v>
@@ -9983,7 +9985,7 @@
         <v>0.13744351846908884</v>
       </c>
       <c r="W160" s="44">
-        <v>0.10027888291084175</v>
+        <v>9.9875160108017558E-2</v>
       </c>
       <c r="X160" s="44">
         <v>0.15362824863350735</v>
@@ -10016,7 +10018,7 @@
         <v>0</v>
       </c>
       <c r="E161" s="44">
-        <v>2.6914642258584892E-2</v>
+        <v>2.6917959872731177E-2</v>
       </c>
       <c r="F161" s="44">
         <v>0</v>
@@ -10190,7 +10192,7 @@
         <v>1</v>
       </c>
       <c r="E163" s="48">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="F163" s="48">
         <v>1</v>
@@ -10244,7 +10246,7 @@
         <v>1</v>
       </c>
       <c r="W163" s="48">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="X163" s="48">
         <v>1</v>

</xml_diff>